<commit_message>
Caching data as much as possible
Close #49
</commit_message>
<xml_diff>
--- a/schema/sheets/Course Planning Data.xlsx
+++ b/schema/sheets/Course Planning Data.xlsx
@@ -36,7 +36,6 @@
     <definedName name="Param_CollegeCounselingOffice">Parameters!$B$7</definedName>
     <definedName localSheetId="8" name="Template_Anchor">'Sample Course Plan'!$B$6</definedName>
     <definedName name="Param_NumOptionsPerDepartment">Parameters!$B$1</definedName>
-    <definedName name="AdvisorList_StudentData">#REF!</definedName>
     <definedName name="Param_CoursePlanTemplate">Parameters!$B$8</definedName>
     <definedName name="Param_NumComments">Parameters!$B$2</definedName>
     <definedName name="Enrollment_Term">'Historical Enrollment'!$R$2</definedName>
@@ -93,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>Number of Options per Department</t>
   </si>
@@ -146,13 +145,16 @@
     <t>Advisor Folder URL</t>
   </si>
   <si>
+    <t>Permissions Set</t>
+  </si>
+  <si>
     <t>ROOT</t>
   </si>
   <si>
-    <t>2MITXPb0E1F1t9tNHMF7nCHGQDWmcRQjc</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/2MITXPb0E1F1t9tNHMF7nCHGQDWmcRQjc</t>
+    <t>FOLDER_ID</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/FOLDER_ID</t>
   </si>
   <si>
     <t>Form</t>
@@ -162,12 +164,6 @@
   </si>
   <si>
     <t>Form Folder URL</t>
-  </si>
-  <si>
-    <t>jyX5tcvxQA2UW3KcmTHcLtvDWy1GWxz8E</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/drive/folders/jyX5tcvxQA2UW3KcmTHcLtvDWy1GWxz8E</t>
   </si>
   <si>
     <t>Student Email</t>
@@ -917,6 +913,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.63"/>
+    <col customWidth="1" min="11" max="11" width="15.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -956,6 +953,14 @@
       <c r="J1" s="1" t="str">
         <f t="array" ref="J1:J2">ifna(if(row(J:J)=1,'Advisor List'!H1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-2,false)),)</f>
         <v>Advisor Last Name</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f t="array" ref="K1:K2">ifna(if(row(K:K)=1,'Advisor Folder Inventory'!B:B,vlookup($H:$H,'Advisor Folder Inventory'!$A:$B,2,false)),)</f>
+        <v>Advisor Folder ID</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f t="array" ref="L1:L2">ifna(if(row(L:L)=1,'Form Folder Inventory'!C:C,vlookup($G:$G,'Form Folder Inventory'!$A:$B,2,false)),)</f>
+        <v>Form Folder URL</v>
       </c>
     </row>
     <row r="2">
@@ -967,6 +972,8 @@
       <c r="H2" s="3"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1007,19 +1014,25 @@
         <f t="array" ref="E1:E2">ifna(if(row(E:E)=1,'Advisor List'!H1,vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false)),)</f>
         <v>Advisor Last Name</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
+      <c r="F2" s="5" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1044,24 +1057,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1093,61 +1106,61 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2">
@@ -1192,25 +1205,25 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1238,31 +1251,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2">
@@ -1307,37 +1320,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2">
@@ -1407,7 +1420,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1417,7 +1430,7 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1436,42 +1449,42 @@
     <row r="4">
       <c r="A4" s="13"/>
       <c r="B4" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="E4" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="13"/>
       <c r="B5" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""English""),2,true,1,true),,1))),)"),"")</f>
@@ -1493,7 +1506,7 @@
     </row>
     <row r="7">
       <c r="A7" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="20" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""Mathematics and Computer Science""),2,true,1,true),,1))),)"),"")</f>
@@ -1515,7 +1528,7 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""World Language and Culture""),2,true,1,true),,1))),)"),"")</f>
@@ -1537,7 +1550,7 @@
     </row>
     <row r="9">
       <c r="A9" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="20" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""Classics""),2,true,1,true),,1))),)"),"")</f>
@@ -1559,7 +1572,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""Science""),2,true,1,true),,1))),)"),"")</f>
@@ -1581,7 +1594,7 @@
     </row>
     <row r="11">
       <c r="A11" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="20" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""Philosophy and Religious Studies""),2,true,1,true),,1))),)"),"")</f>
@@ -1603,7 +1616,7 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""History and Social Science""),2,true,1,true),,1))),)"),"")</f>
@@ -1625,7 +1638,7 @@
     </row>
     <row r="13">
       <c r="A13" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="20" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""Theater and Dance""),2,true,1,true),,1))),)"),"")</f>
@@ -1647,7 +1660,7 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""Visual Arts""),2,true,1,true),,1))),)"),"")</f>
@@ -1669,7 +1682,7 @@
     </row>
     <row r="15">
       <c r="A15" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="20" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""Music""),2,true,1,true),,1))),)"),"")</f>
@@ -1691,7 +1704,7 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Host_ID=""A61003"",Enrollment_Year=""2019 - 2020"",Enrollment_Department=""Non-Departmental""),2,true,1,true),,1))),)"),"")</f>
@@ -1722,7 +1735,7 @@
     <row r="18">
       <c r="A18" s="21"/>
       <c r="B18" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
@@ -1732,15 +1745,15 @@
     <row r="19">
       <c r="A19" s="19"/>
       <c r="B19" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>73</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>74</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
       <c r="F19" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20">
@@ -1770,7 +1783,7 @@
     <row r="23">
       <c r="A23" s="21"/>
       <c r="B23" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
@@ -1780,15 +1793,15 @@
     <row r="24">
       <c r="A24" s="19"/>
       <c r="B24" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="24" t="s">
         <v>73</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>74</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="25"/>
       <c r="F24" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25">
@@ -1818,7 +1831,7 @@
     <row r="28">
       <c r="A28" s="21"/>
       <c r="B28" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
@@ -1828,15 +1841,15 @@
     <row r="29">
       <c r="A29" s="19"/>
       <c r="B29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="24" t="s">
         <v>73</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>74</v>
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="25"/>
       <c r="F29" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30">

</xml_diff>

<commit_message>
Reconfigured course title extraction
Closes #78. Will wait to run updates until later in the day in case there are different available courses.
</commit_message>
<xml_diff>
--- a/schema/sheets/Course Planning Data.xlsx
+++ b/schema/sheets/Course Planning Data.xlsx
@@ -17,8 +17,8 @@
   <definedNames>
     <definedName name="Enrollment_Title">'Historical Enrollment'!$X$2</definedName>
     <definedName name="Param_FormFolderNameFormat">Parameters!$B$3</definedName>
+    <definedName name="Enrollment_Include">'Historical Enrollment'!$Y$2</definedName>
     <definedName name="Course_ID">'Course List'!$A$2</definedName>
-    <definedName name="Enrollment_Include">'Historical Enrollment'!$Y$2</definedName>
     <definedName name="Enrollment_Original_Title">'Historical Enrollment'!$I$2</definedName>
     <definedName name="Enrollment_Year">'Historical Enrollment'!$G$2</definedName>
     <definedName name="Course_Available">'Course List'!$K$2</definedName>
@@ -54,7 +54,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">Last updated from "Historical Enrollment for Course Planning" 3/8/2023, 1:46:34 PM</t>
+        <t xml:space="preserve">Last updated from "Historical Enrollment for Course Planning" 3/30/2023, 10:58:44 AM</t>
       </text>
     </comment>
   </commentList>
@@ -84,7 +84,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">Last updated from "Course List" 3/24/2023, 10:08:01 AM</t>
+        <t xml:space="preserve">Last updated from "Course List" 3/31/2023, 8:52:02 AM</t>
       </text>
     </comment>
   </commentList>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
   <si>
     <t>Cell Color Legend</t>
   </si>
@@ -459,7 +459,7 @@
     <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -512,7 +512,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -523,6 +523,35 @@
           <fgColor rgb="FFCC0000"/>
           <bgColor rgb="FFCC0000"/>
         </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
       </fill>
       <border/>
     </dxf>
@@ -875,154 +904,187 @@
     </row>
     <row r="2">
       <c r="A2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=A1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=A1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
       <c r="B2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=B1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=B1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
       <c r="C2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=C1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=C1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
       <c r="D2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=D1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=D1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
       <c r="E2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=E1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=E1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
       <c r="F2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=F1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=F1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
       <c r="G2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=G1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=G1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
       <c r="H2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=H1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=H1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
       <c r="I2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=I1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=I1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
       <c r="J2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=J1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=J1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
       <c r="K2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I31,Course_Department=K1,Course_Available),3,true,1,true),,4));""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=K1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="B3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="C3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="D3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="E3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="F3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="G3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="H3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="I3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="J3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="K3" s="31" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="B3" s="31" t="str">
+      <c r="B4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="C3" s="31" t="str">
+      <c r="C4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="D3" s="31" t="str">
+      <c r="D4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="E3" s="31" t="str">
+      <c r="E4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="F3" s="31" t="str">
+      <c r="F4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="G3" s="31" t="str">
+      <c r="G4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="H3" s="31" t="str">
+      <c r="H4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="I3" s="31" t="str">
+      <c r="I4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="J3" s="31" t="str">
+      <c r="J4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="K3" s="31" t="str">
+      <c r="K4" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="31" t="str">
+    <row r="5">
+      <c r="A5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="B4" s="31" t="str">
+      <c r="B5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="C4" s="31" t="str">
+      <c r="C5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="D4" s="31" t="str">
+      <c r="D5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="E4" s="31" t="str">
+      <c r="E5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="F4" s="31" t="str">
+      <c r="F5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="G4" s="31" t="str">
+      <c r="G5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="H4" s="31" t="str">
+      <c r="H5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="I4" s="31" t="str">
+      <c r="I5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="J4" s="31" t="str">
+      <c r="J5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="K4" s="31" t="str">
+      <c r="K5" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
     </row>
     <row r="6">
       <c r="A6" s="31"/>
@@ -1361,6 +1423,71 @@
       <c r="I31" s="31"/>
       <c r="J31" s="31"/>
       <c r="K31" s="31"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="31"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1483,9 +1610,9 @@
     <col customWidth="1" min="4" max="4" width="27.88"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="12" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ifna(""Missing: ""&amp;filter(Course_Title,isna(Course_Available)),""All courses synced from Blackbaud are available in this list"")"),"Missing: ")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ifna(""Missing: ""&amp;join("", "",filter(Course_Title,isna(Course_Available))),""All courses synced from Blackbaud are shown in this list. Scan the list for red/yellow highlighted duplicates if necessary."")"),"Missing: ")</f>
         <v>Missing: </v>
       </c>
     </row>
@@ -1524,14 +1651,13 @@
       <c r="E3" s="17" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F3" s="7" t="b">
-        <v>1</v>
-      </c>
+      <c r="F3" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$2:$F$3">
     <sortState ref="A2:F3">
       <sortCondition ref="D2:D3"/>
+      <sortCondition ref="B2:B3"/>
       <sortCondition ref="C2:C3"/>
     </sortState>
   </autoFilter>
@@ -1541,6 +1667,16 @@
   <conditionalFormatting sqref="A1:F1">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>left($A1,7)="Missing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:F3">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>and(countif($A$1:$A2,$A3),not($F3))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:F3">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>and(countif($A$1:$A2,$A3),$F3)</formula>
     </cfRule>
   </conditionalFormatting>
   <drawing r:id="rId1"/>
@@ -1968,8 +2104,9 @@
       <c r="E1" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>52</v>
+      <c r="F1" s="18" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(F:F)=1,""Course Title"",iferror(index(REGEXEXTRACT(C:C,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
+        <v>Course Title</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>60</v>
@@ -1995,10 +2132,7 @@
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
-      <c r="F2" s="30" t="str">
-        <f t="array" ref="F2">iferror(left(C2,find(" (",C2)-1),C2)</f>
-        <v/>
-      </c>
+      <c r="F2" s="30"/>
       <c r="G2" s="30" t="str">
         <f t="array" ref="G2">SWITCH(right(C2,3),"(F)","Fall","(W)","Winter","(S)","Spring",)</f>
         <v/>
@@ -2020,6 +2154,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:K2">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>not($K2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Prep for student folders
Working on #80. Restructured shared folder, permissions. Updated documentation to reflect changes.
</commit_message>
<xml_diff>
--- a/schema/sheets/Course Planning Data.xlsx
+++ b/schema/sheets/Course Planning Data.xlsx
@@ -7,18 +7,20 @@
     <sheet state="visible" name="Parameters" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Available Courses" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Course Plan Inventory" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Advisor Folder Inventory" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Form Folder Inventory" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Historical Enrollment" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Advisor List" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Course List" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="Courses by Department" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="Student Folder Inventory" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Advisor Folder Inventory" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Plans Form Folder Inventory" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Folders Form Folder Inventory" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="Historical Enrollment" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Advisor List" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="Course List" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="Courses by Department" sheetId="12" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="Enrollment_Title">'Historical Enrollment'!$X$2</definedName>
     <definedName name="Param_FormFolderNameFormat">Parameters!$B$3</definedName>
+    <definedName name="Enrollment_Include">'Historical Enrollment'!$Y$2</definedName>
     <definedName name="Course_ID">'Course List'!$A$2</definedName>
-    <definedName name="Enrollment_Include">'Historical Enrollment'!$Y$2</definedName>
     <definedName name="Enrollment_Original_Title">'Historical Enrollment'!$I$2</definedName>
     <definedName name="Enrollment_Year">'Historical Enrollment'!$G$2</definedName>
     <definedName name="Course_Available">'Course List'!$K$2</definedName>
@@ -39,8 +41,8 @@
     <definedName name="Enrollment_BaseTitle">'Historical Enrollment'!$U$2</definedName>
     <definedName name="Param_AdvisorFolderNameFormat">Parameters!$B$4</definedName>
     <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'Available Courses'!$A$2:$F$3</definedName>
-    <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">'Historical Enrollment'!$A$1:$Y$2</definedName>
-    <definedName hidden="1" localSheetId="7" name="_xlnm._FilterDatabase">'Advisor List'!$A$1:$H$2</definedName>
+    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'Historical Enrollment'!$A$1:$Y$2</definedName>
+    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">'Advisor List'!$A$1:$H$2</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -92,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
   <si>
     <t>Cell Color Legend</t>
   </si>
@@ -172,6 +174,18 @@
     <t>Course Plan URL</t>
   </si>
   <si>
+    <t>Student Folder</t>
+  </si>
+  <si>
+    <t>Student Folder ID</t>
+  </si>
+  <si>
+    <t>Student Folder URL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>Advisor Email</t>
   </si>
   <si>
@@ -200,6 +214,12 @@
   </si>
   <si>
     <t>Form Folder URL</t>
+  </si>
+  <si>
+    <t>Folder ID</t>
+  </si>
+  <si>
+    <t>Folder URL</t>
   </si>
   <si>
     <t>Student Email</t>
@@ -315,7 +335,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -355,6 +375,13 @@
     <font>
       <i/>
       <color rgb="FFB7B7B7"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -407,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -465,6 +492,7 @@
     <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -480,7 +508,9 @@
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -501,7 +531,6 @@
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
@@ -509,7 +538,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <font>
         <b/>
@@ -545,6 +574,19 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD966"/>
+          <bgColor rgb="FFFFD966"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFCCCCCC"/>
       </font>
       <fill>
@@ -561,6 +603,14 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -860,631 +910,961 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="$A$1:$H$2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="8" max="11" width="15.13"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="18" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(F:F)=1,""Course Title"",iferror(index(REGEXEXTRACT(C:C,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
+        <v>Course Title</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="18" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula(if(row(E:E)=1,""Formatted Description"",trim(REGEXREPLACE(SUBSTITUTE(substitute(E:E,""&lt;br /&gt;"",char(10)),""&amp;#160;"","" ""),""&lt;\/\w+&gt;|&lt;\w+.*?&gt;"",""""))))"),"Formatted Description")</f>
+        <v>Formatted Description</v>
+      </c>
+      <c r="K1" s="18" t="str">
+        <f t="array" ref="K1:K2">if(row(K:K)=1,"Available",vlookup(A:A,'Available Courses'!A2:F$3,6,false))</f>
+        <v>Available</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33" t="str">
+        <f t="array" ref="G2">SWITCH(right(C2,3),"(F)","Fall","(W)","Winter","(S)","Spring",)</f>
+        <v/>
+      </c>
+      <c r="H2" s="26">
+        <f t="array" ref="H2">switch(G2,"Fall",1,"Winter",2,"Spring",3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="26" t="str">
+        <f t="array" ref="I2">if(G2&lt;&gt;"",if(countif(Course_Title,F2&amp;" (Y)"),,F2&amp;" ("&amp;G2&amp;")"),F2)</f>
+        <v/>
+      </c>
+      <c r="J2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
+      </c>
+      <c r="K2" s="26" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:K2">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>not($K2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="15.13"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=A1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="A2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=A1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="B2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=B1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="B2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=B1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="C2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=C1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="C2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=C1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="D2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=D1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="D2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=D1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="E2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=E1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="E2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=E1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="F2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=F1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="F2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=F1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="G2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=G1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="G2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=G1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="H2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=H1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="H2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=H1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="I2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=I1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="I2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=I1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="J2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=J1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="J2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=J1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="K2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I36,Course_Department=K1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="K2" s="26" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=K1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="31" t="str">
+      <c r="A3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="B3" s="31" t="str">
+      <c r="B3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="C3" s="31" t="str">
+      <c r="C3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="D3" s="31" t="str">
+      <c r="D3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="E3" s="31" t="str">
+      <c r="E3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="F3" s="31" t="str">
+      <c r="F3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="G3" s="31" t="str">
+      <c r="G3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="H3" s="31" t="str">
+      <c r="H3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="I3" s="31" t="str">
+      <c r="I3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="J3" s="31" t="str">
+      <c r="J3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="K3" s="31" t="str">
+      <c r="K3" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="31" t="str">
+      <c r="A4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="B4" s="31" t="str">
+      <c r="B4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="C4" s="31" t="str">
+      <c r="C4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="D4" s="31" t="str">
+      <c r="D4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="E4" s="31" t="str">
+      <c r="E4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="F4" s="31" t="str">
+      <c r="F4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="G4" s="31" t="str">
+      <c r="G4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="H4" s="31" t="str">
+      <c r="H4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="I4" s="31" t="str">
+      <c r="I4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="J4" s="31" t="str">
+      <c r="J4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="K4" s="31" t="str">
+      <c r="K4" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="31" t="str">
+      <c r="A5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="B5" s="31" t="str">
+      <c r="B5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="C5" s="31" t="str">
+      <c r="C5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="D5" s="31" t="str">
+      <c r="D5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="E5" s="31" t="str">
+      <c r="E5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="F5" s="31" t="str">
+      <c r="F5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="G5" s="31" t="str">
+      <c r="G5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="H5" s="31" t="str">
+      <c r="H5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="I5" s="31" t="str">
+      <c r="I5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="J5" s="31" t="str">
+      <c r="J5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="K5" s="31" t="str">
+      <c r="K5" s="26" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="11">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
     </row>
     <row r="14">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
     </row>
     <row r="16">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
     </row>
     <row r="17">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
     </row>
     <row r="18">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
     </row>
     <row r="20">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
     </row>
     <row r="22">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
     </row>
     <row r="23">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
     </row>
     <row r="24">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
     </row>
     <row r="25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
     </row>
     <row r="26">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
     </row>
     <row r="27">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
     </row>
     <row r="28">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
     </row>
     <row r="29">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
     </row>
     <row r="30">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
     </row>
     <row r="31">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
     </row>
     <row r="32">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
     </row>
     <row r="33">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
     </row>
     <row r="34">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
     </row>
     <row r="35">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
     </row>
     <row r="36">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1613,7 +1993,7 @@
         <v>Missing: </v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
@@ -1678,6 +2058,11 @@
       <formula>and(countif($A$1:$A2,$A3),$F3)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A3:F3">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>isna($B3)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1696,7 +2081,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.63"/>
-    <col customWidth="1" min="11" max="11" width="15.13"/>
+    <col customWidth="1" min="12" max="12" width="15.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1726,39 +2111,50 @@
         <v>Grad Year</v>
       </c>
       <c r="H1" s="19" t="str">
-        <f t="array" ref="H1:H2">ifna(if(row(H:H)=1,'Advisor List'!F1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-2,false)),)</f>
+        <f t="array" ref="H1:H2">ifna(if(row(H:H)=1,'Student Folder Inventory'!B1,vlookup($A:$A,'Student Folder Inventory'!$A:$B,2,false)),)</f>
+        <v>Student Folder ID</v>
+      </c>
+      <c r="I1" s="20" t="str">
+        <f t="array" ref="I1:I2">ifna(if(row(I:I)=1,'Advisor List'!F1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-3,false)),)</f>
         <v>Advisor Email</v>
       </c>
-      <c r="I1" s="18" t="str">
-        <f t="array" ref="I1:I2">ifna(if(row(I:I)=1,'Advisor List'!G1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-2,false)),)</f>
+      <c r="J1" s="18" t="str">
+        <f t="array" ref="J1:J2">ifna(if(row(J:J)=1,'Advisor List'!G1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-3,false)),)</f>
         <v>Advisor First Name</v>
       </c>
-      <c r="J1" s="18" t="str">
-        <f t="array" ref="J1:J2">ifna(if(row(J:J)=1,'Advisor List'!H1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-2,false)),)</f>
+      <c r="K1" s="18" t="str">
+        <f t="array" ref="K1:K2">ifna(if(row(K:K)=1,'Advisor List'!H1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-3,false)),)</f>
         <v>Advisor Last Name</v>
       </c>
-      <c r="K1" s="18" t="str">
-        <f t="array" ref="K1:K2">ifna(if(row(K:K)=1,'Advisor Folder Inventory'!B1,vlookup($H:$H,'Advisor Folder Inventory'!$A:$B,2,false)),)</f>
+      <c r="L1" s="18" t="str">
+        <f t="array" ref="L1:L2">ifna(if(row(L:L)=1,'Advisor Folder Inventory'!B1,vlookup($I:$I,'Advisor Folder Inventory'!$A:$B,2,false)),)</f>
         <v>Advisor Folder ID</v>
       </c>
-      <c r="L1" s="18" t="str">
-        <f t="array" ref="L1:L2">ifna(if(row(L:L)=1,'Form Folder Inventory'!B1,vlookup($G:$G,'Form Folder Inventory'!$A:$B,2,false)),)</f>
+      <c r="M1" s="18" t="str">
+        <f t="array" ref="M1:M2">ifna(if(row(M:M)=1,'Plans Form Folder Inventory'!B1,vlookup($G:$G,'Plans Form Folder Inventory'!$A:$B,2,false)),)</f>
         <v>Form Folder ID</v>
       </c>
+      <c r="N1" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="23"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1766,6 +2162,61 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="25" t="str">
+        <f t="array" ref="D1:D2">if($A:$A&lt;&gt;"",vlookup($A:$A,'Advisor List'!$A:$D,2,false),"")</f>
+        <v>Student Email</v>
+      </c>
+      <c r="E1" s="25" t="str">
+        <f t="array" ref="E1:E2">if($A:$A&lt;&gt;"",vlookup($A:$A,'Advisor List'!$A:$D,3,false),"")</f>
+        <v>Student First Name</v>
+      </c>
+      <c r="F1" s="25" t="str">
+        <f t="array" ref="F1:F2">if($A:$A&lt;&gt;"",vlookup($A:$A,'Advisor List'!$A:$D,4,false),"")</f>
+        <v>Student Last Name</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1783,13 +2234,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D1" s="18" t="str">
         <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!G1,vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false)),)</f>
@@ -1800,22 +2251,22 @@
         <v>Advisor Last Name</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="21" t="b">
+      <c r="A2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1827,7 +2278,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1842,24 +2293,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="B2" s="21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>32</v>
+      <c r="C2" s="27" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1870,7 +2321,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1890,119 +2384,119 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="C1" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="25" t="s">
+      <c r="J1" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="25" t="s">
+      <c r="M1" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="R1" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="S1" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>51</v>
+      <c r="Q1" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="U1" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(U:U)=1,""Course Title"",iferror(index(REGEXEXTRACT(I:I,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
         <v>Course Title</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="X1" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y1" s="26" t="str">
+        <v>60</v>
+      </c>
+      <c r="Y1" s="29" t="str">
         <f t="array" ref="Y1:Y2">if(row(Y:Y)=1,"Include",not((((H:H=6100)+(H:H=6130)+(H:H=6132))*(P:P="Philosophy and Religious Studies"))))</f>
         <v>Include</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30" t="str">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33" t="str">
         <f t="array" ref="V2">SWITCH(right(Enrollment_TitleWithTerm,3),"(F)","Fall","(W)","Winter","(S)","Spring",)</f>
         <v/>
       </c>
-      <c r="W2" s="31">
+      <c r="W2" s="26">
         <f t="array" ref="W2">switch(Enrollment_Term,"Fall",1,"Winter",2,"Spring",3,0)-if(Enrollment_Dropped,0.5,0)</f>
         <v>0</v>
       </c>
-      <c r="X2" s="31" t="str">
+      <c r="X2" s="26" t="str">
         <f t="array" ref="X2">if(Enrollment_Term&lt;&gt;"",if(countif(Enrollment_Original_Title,Enrollment_BaseTitle&amp;" (Y)"),,Enrollment_BaseTitle&amp;" ("&amp;Enrollment_Term&amp;")"),Enrollment_BaseTitle)&amp;if(Enrollment_Dropped," (Dropped)","")</f>
         <v/>
       </c>
-      <c r="Y2" s="31" t="b">
+      <c r="Y2" s="26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2011,152 +2505,4 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="$A$1:$H$2"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="8" max="11" width="15.13"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="18" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(F:F)=1,""Course Title"",iferror(index(REGEXEXTRACT(C:C,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
-        <v>Course Title</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="18" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula(if(row(E:E)=1,""Formatted Description"",trim(REGEXREPLACE(SUBSTITUTE(substitute(E:E,""&lt;br /&gt;"",char(10)),""&amp;#160;"","" ""),""&lt;\/\w+&gt;|&lt;\w+.*?&gt;"",""""))))"),"Formatted Description")</f>
-        <v>Formatted Description</v>
-      </c>
-      <c r="K1" s="18" t="str">
-        <f t="array" ref="K1:K2">if(row(K:K)=1,"Available",vlookup(A:A,'Available Courses'!A2:F$3,6,false))</f>
-        <v>Available</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30" t="str">
-        <f t="array" ref="G2">SWITCH(right(C2,3),"(F)","Fall","(W)","Winter","(S)","Spring",)</f>
-        <v/>
-      </c>
-      <c r="H2" s="31">
-        <f t="array" ref="H2">switch(G2,"Fall",1,"Winter",2,"Spring",3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="31" t="str">
-        <f t="array" ref="I2">if(G2&lt;&gt;"",if(countif(Course_Title,F2&amp;" (Y)"),,F2&amp;" ("&amp;G2&amp;")"),F2)</f>
-        <v/>
-      </c>
-      <c r="J2" s="31" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
-        <v/>
-      </c>
-      <c r="K2" s="31" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:K2">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>not($K2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Create student folders with plan
For all _new_ course plans. #80
</commit_message>
<xml_diff>
--- a/schema/sheets/Course Planning Data.xlsx
+++ b/schema/sheets/Course Planning Data.xlsx
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
   <si>
     <t>Cell Color Legend</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Course Plan URL</t>
-  </si>
-  <si>
-    <t>Student Folder</t>
   </si>
   <si>
     <t>Student Folder ID</t>
@@ -916,25 +913,25 @@
         <v>23</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>45</v>
-      </c>
       <c r="E1" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="28" t="s">
+      <c r="H1" s="28" t="s">
         <v>62</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -975,7 +972,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="28" t="s">
         <v>19</v>
@@ -984,20 +981,20 @@
         <v>20</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(F:F)=1,""Course Title"",iferror(index(REGEXEXTRACT(C:C,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
         <v>Course Title</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>60</v>
       </c>
       <c r="J1" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula(if(row(E:E)=1,""Formatted Description"",trim(REGEXREPLACE(SUBSTITUTE(substitute(E:E,""&lt;br /&gt;"",char(10)),""&amp;#160;"","" ""),""&lt;\/\w+&gt;|&lt;\w+.*?&gt;"",""""))))"),"Formatted Description")</f>
@@ -1064,37 +1061,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>75</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2">
@@ -2134,9 +2131,6 @@
         <f t="array" ref="M1:M2">ifna(if(row(M:M)=1,'Plans Form Folder Inventory'!B1,vlookup($G:$G,'Plans Form Folder Inventory'!$A:$B,2,false)),)</f>
         <v>Form Folder ID</v>
       </c>
-      <c r="N1" s="9" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="21"/>
@@ -2152,9 +2146,6 @@
       <c r="K2" s="23"/>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
-      <c r="N2" s="22" t="b">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2179,10 +2170,10 @@
         <v>23</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="D1" s="25" t="str">
         <f t="array" ref="D1:D2">if($A:$A&lt;&gt;"",vlookup($A:$A,'Advisor List'!$A:$D,2,false),"")</f>
@@ -2202,13 +2193,13 @@
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
       <c r="D2" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2234,13 +2225,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>32</v>
       </c>
       <c r="D1" s="18" t="str">
         <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!G1,vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false)),)</f>
@@ -2251,18 +2242,18 @@
         <v>Advisor Last Name</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="27" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>36</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -2293,24 +2284,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="27" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2336,24 +2327,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="27" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2388,74 +2379,74 @@
         <v>23</v>
       </c>
       <c r="B1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="G1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="H1" s="28" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>48</v>
       </c>
       <c r="I1" s="28" t="s">
         <v>19</v>
       </c>
       <c r="J1" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="28" t="s">
         <v>49</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>50</v>
       </c>
       <c r="L1" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="O1" s="28" t="s">
         <v>52</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>53</v>
       </c>
       <c r="P1" s="28" t="s">
         <v>20</v>
       </c>
       <c r="Q1" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="S1" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>56</v>
-      </c>
-      <c r="T1" s="28" t="s">
-        <v>57</v>
       </c>
       <c r="U1" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(U:U)=1,""Course Title"",iferror(index(REGEXEXTRACT(I:I,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
         <v>Course Title</v>
       </c>
       <c r="V1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="W1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="X1" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="X1" s="18" t="s">
-        <v>60</v>
       </c>
       <c r="Y1" s="29" t="str">
         <f t="array" ref="Y1:Y2">if(row(Y:Y)=1,"Include",not((((H:H=6100)+(H:H=6130)+(H:H=6132))*(P:P="Philosophy and Religious Studies"))))</f>

</xml_diff>

<commit_message>
Restructured export from Bb
Haven’t documented the schema yet (although the manual process is described in #77). The revision will let me eventually resolve both #75 and #77, as well as setting me up to implement [this comment](https://github.com/groton-school/course-planning-tool/issues/72#issuecomment-1496340236) in #72
</commit_message>
<xml_diff>
--- a/schema/sheets/Course Planning Data.xlsx
+++ b/schema/sheets/Course Planning Data.xlsx
@@ -11,59 +11,49 @@
     <sheet state="visible" name="Advisor Folder Inventory" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="Plans Form Folder Inventory" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Folders Form Folder Inventory" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Historical Enrollment" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="Advisor List" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="Course List" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="Courses by Department" sheetId="12" r:id="rId15"/>
+    <sheet state="visible" name="Advisor List" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Course List" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="Courses by Department" sheetId="11" r:id="rId14"/>
+    <sheet state="visible" name="Historical Enrollment" sheetId="12" r:id="rId15"/>
+    <sheet state="visible" name="Individual Enrollment History" sheetId="13" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="Enrollment_Title">'Historical Enrollment'!$X$2</definedName>
+    <definedName name="Enrollment_Title">'Historical Enrollment'!$S:$S</definedName>
     <definedName name="Param_FormFolderNameFormat">Parameters!$B$3</definedName>
-    <definedName name="Enrollment_Include">'Historical Enrollment'!$Y$2</definedName>
+    <definedName name="Param_StudentFolderNameFormat">Parameters!$B$4</definedName>
+    <definedName name="Enrollment_CourseCode">'Historical Enrollment'!$G:$G</definedName>
     <definedName name="Course_ID">'Course List'!$A$2</definedName>
-    <definedName name="Enrollment_Original_Title">'Historical Enrollment'!$I$2</definedName>
-    <definedName name="Enrollment_Year">'Historical Enrollment'!$G$2</definedName>
     <definedName name="Course_Available">'Course List'!$K$2</definedName>
-    <definedName name="Param_CollegeCounselingOffice">Parameters!$B$7</definedName>
-    <definedName name="Enrollment_TitleWithTerm">'Historical Enrollment'!$I$2</definedName>
-    <definedName name="Param_CoursePlanNameFormat">Parameters!$B$5</definedName>
-    <definedName name="Enrollment_Dropped">'Historical Enrollment'!$S$2</definedName>
-    <definedName name="Enrollment_Order">'Historical Enrollment'!$W$2</definedName>
+    <definedName name="IEH_GradYear">'Individual Enrollment History'!$C$2</definedName>
+    <definedName name="Param_CoursePlanNameFormat">Parameters!$B$6</definedName>
+    <definedName name="Enrollment_Order">'Historical Enrollment'!$R:$R</definedName>
+    <definedName name="Enrollment_Host_ID">'Historical Enrollment'!$A:$A</definedName>
+    <definedName name="Course_Department">'Course List'!$D$2</definedName>
+    <definedName name="Param_StudiesCommittee">Parameters!$B$7</definedName>
+    <definedName name="Enrollment_Department">'Historical Enrollment'!$P:$P</definedName>
+    <definedName name="Param_AdvisorFolderNameFormat">Parameters!$B$5</definedName>
+    <definedName name="Enrollment_Include">'Historical Enrollment'!$T:$T</definedName>
+    <definedName name="Enrollment_Year">'Historical Enrollment'!$F:$F</definedName>
+    <definedName name="IEH_HostID">'Individual Enrollment History'!$B$2</definedName>
+    <definedName name="Param_CollegeCounselingOffice">Parameters!$B$8</definedName>
+    <definedName name="Enrollment_TitleWithTerm">'Historical Enrollment'!$H:$H</definedName>
+    <definedName name="Enrollment_Status">'Historical Enrollment'!$N:$N</definedName>
+    <definedName name="Enrollment_Type">'Historical Enrollment'!$M:$M</definedName>
     <definedName name="Param_NumOptionsPerDepartment">Parameters!$B$1</definedName>
-    <definedName name="Param_CoursePlanTemplate">Parameters!$B$8</definedName>
-    <definedName name="Enrollment_Host_ID">'Historical Enrollment'!$A$2</definedName>
+    <definedName name="Param_CoursePlanTemplate">Parameters!$B$9</definedName>
     <definedName name="Param_NumComments">Parameters!$B$2</definedName>
-    <definedName name="Course_Department">'Course List'!$D$2</definedName>
-    <definedName name="Enrollment_Term">'Historical Enrollment'!$V$2</definedName>
-    <definedName name="Param_StudiesCommittee">Parameters!$B$6</definedName>
-    <definedName name="Enrollment_Department">'Historical Enrollment'!$P$2</definedName>
+    <definedName name="Enrollment_Term">'Historical Enrollment'!$Q:$Q</definedName>
     <definedName name="Course_Title">'Course List'!$C$2</definedName>
-    <definedName name="Enrollment_BaseTitle">'Historical Enrollment'!$U$2</definedName>
-    <definedName name="Param_AdvisorFolderNameFormat">Parameters!$B$4</definedName>
+    <definedName name="Enrollment_BaseTitle">'Historical Enrollment'!$O:$O</definedName>
     <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'Available Courses'!$A$2:$F$3</definedName>
-    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'Historical Enrollment'!$A$1:$Y$2</definedName>
-    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">'Advisor List'!$A$1:$H$2</definedName>
+    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'Advisor List'!$A$1:$I$2</definedName>
+    <definedName hidden="1" localSheetId="11" name="_xlnm._FilterDatabase">'Historical Enrollment'!$A$1:$T$2</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="A1">
-      <text>
-        <t xml:space="preserve">Last updated from "Historical Enrollment for Course Planning" 4/3/2023, 11:38:09 AM</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -78,7 +68,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -94,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
   <si>
     <t>Cell Color Legend</t>
   </si>
@@ -129,6 +119,12 @@
     <t>Class of {{gradYear}}</t>
   </si>
   <si>
+    <t>Student Folder Name Format</t>
+  </si>
+  <si>
+    <t>{{lastName}}, {{firstName}} ‘{{abbrevGradYear}}</t>
+  </si>
+  <si>
     <t>Advisor Folder Name Format</t>
   </si>
   <si>
@@ -222,117 +218,143 @@
     <t>Student Email</t>
   </si>
   <si>
-    <t>Student User ID</t>
-  </si>
-  <si>
     <t>Student First Name</t>
   </si>
   <si>
     <t>Student Last Name</t>
   </si>
   <si>
-    <t>Student Grad Year</t>
-  </si>
-  <si>
-    <t>School Year</t>
+    <t>Grad Year</t>
+  </si>
+  <si>
+    <t>Advisor First Name</t>
+  </si>
+  <si>
+    <t>Advisor Last Name</t>
+  </si>
+  <si>
+    <t>,  ’-2000 []</t>
   </si>
   <si>
     <t>Course Code</t>
   </si>
   <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Group Identifier</t>
-  </si>
-  <si>
-    <t>Faculty User ID</t>
-  </si>
-  <si>
-    <t>Faculty First Name</t>
-  </si>
-  <si>
-    <t>Faculty Last Name</t>
-  </si>
-  <si>
-    <t>Begin Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
-    <t>Dropped</t>
-  </si>
-  <si>
-    <t>Dropped Comment</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Course Term</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Formatted Course Title</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Mathematics and Computer Science</t>
+  </si>
+  <si>
+    <t>World Language and Culture</t>
+  </si>
+  <si>
+    <t>Classics</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Philosophy and Religious Studies</t>
+  </si>
+  <si>
+    <t>History and Social Science</t>
+  </si>
+  <si>
+    <t>Theater and Dance</t>
+  </si>
+  <si>
+    <t>Visual Arts</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Non-Departmental</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Graduation year</t>
+  </si>
+  <si>
+    <t>School year</t>
+  </si>
+  <si>
+    <t>Course code</t>
+  </si>
+  <si>
+    <t>Course title</t>
   </si>
   <si>
     <t>Term</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
-    <t>Formatted Course Title</t>
-  </si>
-  <si>
-    <t>Grad Year</t>
-  </si>
-  <si>
-    <t>Advisor First Name</t>
-  </si>
-  <si>
-    <t>Advisor Last Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Course Term</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Mathematics and Computer Science</t>
-  </si>
-  <si>
-    <t>World Language and Culture</t>
-  </si>
-  <si>
-    <t>Classics</t>
-  </si>
-  <si>
-    <t>Science</t>
-  </si>
-  <si>
-    <t>Philosophy and Religious Studies</t>
-  </si>
-  <si>
-    <t>History and Social Science</t>
-  </si>
-  <si>
-    <t>Theater and Dance</t>
-  </si>
-  <si>
-    <t>Visual Arts</t>
-  </si>
-  <si>
-    <t>Music</t>
-  </si>
-  <si>
-    <t>Non-Departmental</t>
+    <t>Section identifier</t>
+  </si>
+  <si>
+    <t>Departments</t>
+  </si>
+  <si>
+    <t>Is incomplete</t>
+  </si>
+  <si>
+    <t>Enrollment type</t>
+  </si>
+  <si>
+    <t>Enrollment status</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Graduation Year</t>
+  </si>
+  <si>
+    <t>Numerical Year</t>
+  </si>
+  <si>
+    <t>II Form</t>
+  </si>
+  <si>
+    <t>III Form</t>
+  </si>
+  <si>
+    <t>IV Form</t>
+  </si>
+  <si>
+    <t>V Form</t>
+  </si>
+  <si>
+    <t>VI Form</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -386,6 +408,19 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -425,13 +460,70 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="48">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -513,23 +605,62 @@
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
+    <xf borderId="0" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,6 +739,10 @@
 </file>
 
 <file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -907,94 +1042,38 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="$A$1:$H$2"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="8" max="11" width="15.13"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="34" t="s">
-        <v>18</v>
+      <c r="A1" s="31" t="s">
+        <v>20</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F1" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(F:F)=1,""Course Title"",iferror(index(REGEXEXTRACT(C:C,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
         <v>Course Title</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J1" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula(if(row(E:E)=1,""Formatted Description"",trim(REGEXREPLACE(SUBSTITUTE(substitute(E:E,""&lt;br /&gt;"",char(10)),""&amp;#160;"","" ""),""&lt;\/\w+&gt;|&lt;\w+.*?&gt;"",""""))))"),"Formatted Description")</f>
@@ -1006,13 +1085,13 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33" t="str">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30" t="str">
         <f t="array" ref="G2">SWITCH(right(C2,3),"(F)","Fall","(W)","Winter","(S)","Spring",)</f>
         <v/>
       </c>
@@ -1043,7 +1122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1061,37 +1140,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2">
@@ -1864,6 +1943,526 @@
       <c r="K50" s="26"/>
     </row>
   </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4.0" ySplit="1.0" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E1" sqref="E1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="E2" sqref="E2" pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="9.38"/>
+    <col customWidth="1" min="8" max="8" width="37.25"/>
+    <col customWidth="1" min="11" max="11" width="27.88"/>
+    <col customWidth="1" min="19" max="19" width="55.38"/>
+    <col customWidth="1" min="20" max="20" width="9.38"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="18" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(O:O)=1,""Course Title"",if(G:G=5741,""Advanced Physics: Electricity and Magnetism"",iferror(index(REGEXEXTRACT(H:H,""^(.+)( \([FWSY]\))$""),0,1),H:H))))"),"Course Title")</f>
+        <v>Course Title</v>
+      </c>
+      <c r="P1" s="18" t="str">
+        <f t="array" ref="P1:P2">if(row(P:P)=1,"Department",if(K:K="History and Social Science | Philosophy and Religious Studies","History and Social Science",K:K))</f>
+        <v>Department</v>
+      </c>
+      <c r="Q1" s="18" t="str">
+        <f t="array" ref="Q1:Q2">if(row(Q:Q)=1,"Term",if(G:G=5741,"Fall, Winter",SWITCH(right(H:H,3),"(F)","Fall","(W)","Winter","(S)","Spring","(Y)", "Year","Year")))</f>
+        <v>Term</v>
+      </c>
+      <c r="R1" s="18" t="str">
+        <f t="array" ref="R1:R2">if(row(R:R)=1,"Order",switch(I:I,"Fall Term",1,"Winter Term",2,"Spring Term",3,0)-if(N:N="Dropped",0.5,0))</f>
+        <v>Order</v>
+      </c>
+      <c r="S1" s="18" t="str">
+        <f t="array" ref="S1:S2">if(row(S:S)=1,"Formatted Course Title",O:O&amp;if((M:M="Audit")+(N:N="Dropped")+((Q:Q&lt;&gt;"Year")*(Q:Q&lt;&gt;""))," ("&amp;if((Q:Q&lt;&gt;"")*(Q:Q&lt;&gt;"Year"),Q:Q,"")&amp;if((Q:Q&lt;&gt;"")*(Q:Q&lt;&gt;"Year")*(M:M="Audit"),", ","")&amp;if(M:M="Audit","Audit","")&amp;If((M:M="Audit")*(N:N="Dropped"),", ","")&amp;if(N:N="Dropped","Dropped","")&amp;")",""))</f>
+        <v>Formatted Course Title</v>
+      </c>
+      <c r="T1" s="32" t="str">
+        <f t="array" ref="T1:T2">if(row(T:T)=1,"Include",(N:N="Enrolled")+((N:N="Dropped")*(countifs(Enrollment_Host_ID,A:A,Enrollment_CourseCode,G:G,Enrollment_Year,F:F,Enrollment_Term,Q:Q,Enrollment_Status,"Enrolled")=0)))</f>
+        <v>Include</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="S2" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="30">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="$A$1:$T$2">
+    <sortState ref="A1:T2">
+      <sortCondition ref="D1:D2"/>
+      <sortCondition ref="C1:C2"/>
+      <sortCondition ref="F1:F2"/>
+      <sortCondition ref="I1:I2"/>
+      <sortCondition ref="P1:P2"/>
+      <sortCondition ref="G1:G2"/>
+    </sortState>
+  </autoFilter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="30.5"/>
+    <col customWidth="1" min="2" max="6" width="22.5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("if(A2&lt;&gt;"""",A2,REGEXEXTRACT(A1,""\[(.+)\]$""))"),"#N/A")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C2" s="38" t="str">
+        <f t="array" ref="C2">INDEX('Advisor List'!E:E,match(B2,'Advisor List'!A:A,0),0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="40" t="str">
+        <f t="array" ref="B3:F3">IEH_GradYear-(6-COLUMN(B5:F5))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C3" s="40" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D3" s="41" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E3" s="41" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F3" s="42" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="43"/>
+      <c r="B4" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="43"/>
+      <c r="B5" s="45" t="str">
+        <f t="array" ref="B5:F5">(B3:F3-1)&amp;" - "&amp;B3:F3</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C5" s="45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" s="45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E5" s="45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F5" s="45" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C6" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D6" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E6" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F6" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C7" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D7" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E7" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F7" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C8" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D8" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E8" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F8" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C9" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D9" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E9" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F9" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C10" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D10" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E10" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F10" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C11" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D11" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E11" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F11" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C12" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D12" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E12" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F12" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C13" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D13" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E13" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F13" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C14" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D14" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E14" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F14" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C15" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D15" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E15" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F15" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="C16" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="D16" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="E16" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+      <c r="F16" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A1">
+      <formula1>'Advisor List'!$I$2:$I16</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1929,33 +2528,41 @@
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="11"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B6:B7">
-      <formula1>IFERROR(ISEMAIL(B6), true)</formula1>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B7:B8">
+      <formula1>IFERROR(ISEMAIL(B7), true)</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B2">
       <formula1>2.0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B3:B5">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B3:B6">
       <formula1>NOT(ISERROR(SEARCH(("{{"),(B3))))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B8">
-      <formula1>IFERROR(ISURL(B8), true)</formula1>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B9">
+      <formula1>IFERROR(ISURL(B9), true)</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B1">
       <formula1>1.0</formula1>
@@ -1992,23 +2599,23 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="14" t="str">
         <f t="array" ref="B2:E3">vlookup($A2:$A3,{'Course List'!$A:$D,'Course List'!$J:$J},column(B:E),false)</f>
         <v>Course Code</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -2083,13 +2690,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" s="18" t="str">
         <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!B1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-2,false)),)</f>
@@ -2167,13 +2774,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D1" s="25" t="str">
         <f t="array" ref="D1:D2">if($A:$A&lt;&gt;"",vlookup($A:$A,'Advisor List'!$A:$D,2,false),"")</f>
@@ -2193,13 +2800,13 @@
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
       <c r="D2" s="26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2225,13 +2832,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D1" s="18" t="str">
         <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!G1,vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false)),)</f>
@@ -2242,18 +2849,18 @@
         <v>Advisor Last Name</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -2284,24 +2891,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2327,24 +2934,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2368,131 +2975,54 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="9" max="9" width="37.25"/>
-    <col customWidth="1" min="16" max="16" width="27.88"/>
-    <col customWidth="1" min="24" max="24" width="55.38"/>
-    <col customWidth="1" min="25" max="25" width="9.38"/>
+    <col customWidth="1" min="9" max="9" width="32.63"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="28" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="I1" s="18" t="str">
+        <f t="array" ref="I1:I2">if(row(I:I)=1,"Menu Option",D:D&amp;", "&amp;C:C&amp;" ’"&amp;(E:E-2000)&amp;" ["&amp;A:A&amp;"]")</f>
+        <v>Menu Option</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="P1" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="S1" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="U1" s="18" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(U:U)=1,""Course Title"",iferror(index(REGEXEXTRACT(I:I,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
-        <v>Course Title</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="X1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y1" s="29" t="str">
-        <f t="array" ref="Y1:Y2">if(row(Y:Y)=1,"Include",not((((H:H=6100)+(H:H=6130)+(H:H=6132))*(P:P="Philosophy and Religious Studies"))))</f>
-        <v>Include</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33" t="str">
-        <f t="array" ref="V2">SWITCH(right(Enrollment_TitleWithTerm,3),"(F)","Fall","(W)","Winter","(S)","Spring",)</f>
-        <v/>
-      </c>
-      <c r="W2" s="26">
-        <f t="array" ref="W2">switch(Enrollment_Term,"Fall",1,"Winter",2,"Spring",3,0)-if(Enrollment_Dropped,0.5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="X2" s="26" t="str">
-        <f t="array" ref="X2">if(Enrollment_Term&lt;&gt;"",if(countif(Enrollment_Original_Title,Enrollment_BaseTitle&amp;" (Y)"),,Enrollment_BaseTitle&amp;" ("&amp;Enrollment_Term&amp;")"),Enrollment_BaseTitle)&amp;if(Enrollment_Dropped," (Dropped)","")</f>
-        <v/>
-      </c>
-      <c r="Y2" s="26" t="b">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$Y$2"/>
+  <autoFilter ref="$A$1:$I$2"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Easier “clean copy” for docs
Also:
  - updated dependencies
  - fixed version number in package
  - started work towards [this comment](https://github.com/groton-school/course-planning-tool/issues/76#issuecomment-1500276937) in #76 (which should improve prospects for #72).
</commit_message>
<xml_diff>
--- a/schema/sheets/Course Planning Data.xlsx
+++ b/schema/sheets/Course Planning Data.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="87">
   <si>
     <t>Cell Color Legend</t>
   </si>
@@ -194,7 +194,7 @@
     <t>ROOT</t>
   </si>
   <si>
-    <t>FOLDER_ID</t>
+    <t>FILE_ID</t>
   </si>
   <si>
     <t>https://drive.google.com/drive/folders/FOLDER_ID</t>
@@ -523,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -578,27 +578,35 @@
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1047,67 +1055,67 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="18" t="str">
+      <c r="F1" s="28" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(F:F)=1,""Course Title"",iferror(index(REGEXEXTRACT(C:C,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
         <v>Course Title</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="18" t="str">
+      <c r="J1" s="28" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula(if(row(E:E)=1,""Formatted Description"",trim(REGEXREPLACE(SUBSTITUTE(substitute(E:E,""&lt;br /&gt;"",char(10)),""&amp;#160;"","" ""),""&lt;\/\w+&gt;|&lt;\w+.*?&gt;"",""""))))"),"Formatted Description")</f>
         <v>Formatted Description</v>
       </c>
-      <c r="K1" s="18" t="str">
+      <c r="K1" s="28" t="str">
         <f t="array" ref="K1:K2">if(row(K:K)=1,"Available",vlookup(A:A,'Available Courses'!A2:F$3,6,false))</f>
         <v>Available</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30" t="str">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32" t="str">
         <f t="array" ref="G2">SWITCH(right(C2,3),"(F)","Fall","(W)","Winter","(S)","Spring",)</f>
         <v/>
       </c>
-      <c r="H2" s="26">
+      <c r="H2" s="27">
         <f t="array" ref="H2">switch(G2,"Fall",1,"Winter",2,"Spring",3,0)</f>
         <v>0</v>
       </c>
-      <c r="I2" s="26" t="str">
+      <c r="I2" s="27" t="str">
         <f t="array" ref="I2">if(G2&lt;&gt;"",if(countif(Course_Title,F2&amp;" (Y)"),,F2&amp;" ("&amp;G2&amp;")"),F2)</f>
         <v/>
       </c>
-      <c r="J2" s="26" t="str">
+      <c r="J2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="K2" s="26" t="e">
+      <c r="K2" s="27" t="e">
         <v>#N/A</v>
       </c>
     </row>
@@ -1139,808 +1147,808 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="28" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="26" t="str">
+      <c r="A2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=A1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=B1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="C2" s="26" t="str">
+      <c r="C2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=C1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="D2" s="26" t="str">
+      <c r="D2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=D1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="E2" s="26" t="str">
+      <c r="E2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=E1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="F2" s="26" t="str">
+      <c r="F2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=F1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="G2" s="26" t="str">
+      <c r="G2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=G1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="H2" s="26" t="str">
+      <c r="H2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=H1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="I2" s="26" t="str">
+      <c r="I2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=I1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="J2" s="26" t="str">
+      <c r="J2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=J1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="K2" s="26" t="str">
+      <c r="K2" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$F$2:$I50,Course_Department=K1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="26" t="str">
+      <c r="A3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="B3" s="26" t="str">
+      <c r="B3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="C3" s="26" t="str">
+      <c r="C3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="D3" s="26" t="str">
+      <c r="D3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="E3" s="26" t="str">
+      <c r="E3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="F3" s="26" t="str">
+      <c r="F3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="G3" s="26" t="str">
+      <c r="G3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="H3" s="26" t="str">
+      <c r="H3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="I3" s="26" t="str">
+      <c r="I3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="J3" s="26" t="str">
+      <c r="J3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="K3" s="26" t="str">
+      <c r="K3" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="26" t="str">
+      <c r="A4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="B4" s="26" t="str">
+      <c r="B4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="C4" s="26" t="str">
+      <c r="C4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="D4" s="26" t="str">
+      <c r="D4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="E4" s="26" t="str">
+      <c r="E4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="F4" s="26" t="str">
+      <c r="F4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="G4" s="26" t="str">
+      <c r="G4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="H4" s="26" t="str">
+      <c r="H4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="I4" s="26" t="str">
+      <c r="I4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="J4" s="26" t="str">
+      <c r="J4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="K4" s="26" t="str">
+      <c r="K4" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="26" t="str">
+      <c r="A5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="B5" s="26" t="str">
+      <c r="B5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="C5" s="26" t="str">
+      <c r="C5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="D5" s="26" t="str">
+      <c r="D5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="E5" s="26" t="str">
+      <c r="E5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="F5" s="26" t="str">
+      <c r="F5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="G5" s="26" t="str">
+      <c r="G5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="H5" s="26" t="str">
+      <c r="H5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="I5" s="26" t="str">
+      <c r="I5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="J5" s="26" t="str">
+      <c r="J5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="K5" s="26" t="str">
+      <c r="K5" s="27" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
     </row>
     <row r="7">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
     </row>
     <row r="13">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
     </row>
     <row r="14">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
     </row>
     <row r="15">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
     </row>
     <row r="16">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
     </row>
     <row r="17">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
     </row>
     <row r="18">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
     </row>
     <row r="19">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
     </row>
     <row r="20">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
     </row>
     <row r="21">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
     </row>
     <row r="22">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
     </row>
     <row r="23">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
     </row>
     <row r="24">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
     </row>
     <row r="25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
     </row>
     <row r="26">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
     </row>
     <row r="27">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
     </row>
     <row r="28">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
     </row>
     <row r="29">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
     </row>
     <row r="30">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
     </row>
     <row r="31">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
     </row>
     <row r="32">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
     </row>
     <row r="33">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
     </row>
     <row r="34">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
     </row>
     <row r="35">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
     </row>
     <row r="36">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
     </row>
     <row r="37">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
     </row>
     <row r="38">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
-      <c r="K38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
     </row>
     <row r="39">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
     </row>
     <row r="40">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
     </row>
     <row r="41">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
     </row>
     <row r="42">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="26"/>
-      <c r="K42" s="26"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
     </row>
     <row r="43">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
     </row>
     <row r="44">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
     </row>
     <row r="45">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
     </row>
     <row r="46">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
     </row>
     <row r="47">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="27"/>
     </row>
     <row r="48">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
     </row>
     <row r="49">
-      <c r="A49" s="26"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
     </row>
     <row r="50">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="26"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="27"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1970,101 +1978,101 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="18" t="str">
+      <c r="O1" s="28" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(O:O)=1,""Course Title"",if(G:G=5741,""Advanced Physics: Electricity and Magnetism"",iferror(index(REGEXEXTRACT(H:H,""^(.+)( \([FWSY]\))$""),0,1),H:H))))"),"Course Title")</f>
         <v>Course Title</v>
       </c>
-      <c r="P1" s="18" t="str">
+      <c r="P1" s="28" t="str">
         <f t="array" ref="P1:P2">if(row(P:P)=1,"Department",if(K:K="History and Social Science | Philosophy and Religious Studies","History and Social Science",K:K))</f>
         <v>Department</v>
       </c>
-      <c r="Q1" s="18" t="str">
+      <c r="Q1" s="28" t="str">
         <f t="array" ref="Q1:Q2">if(row(Q:Q)=1,"Term",if(G:G=5741,"Fall, Winter",SWITCH(right(H:H,3),"(F)","Fall","(W)","Winter","(S)","Spring","(Y)", "Year","Year")))</f>
         <v>Term</v>
       </c>
-      <c r="R1" s="18" t="str">
+      <c r="R1" s="28" t="str">
         <f t="array" ref="R1:R2">if(row(R:R)=1,"Order",switch(I:I,"Fall Term",1,"Winter Term",2,"Spring Term",3,0)-if(N:N="Dropped",0.5,0))</f>
         <v>Order</v>
       </c>
-      <c r="S1" s="18" t="str">
+      <c r="S1" s="28" t="str">
         <f t="array" ref="S1:S2">if(row(S:S)=1,"Formatted Course Title",O:O&amp;if((M:M="Audit")+(N:N="Dropped")+((Q:Q&lt;&gt;"Year")*(Q:Q&lt;&gt;""))," ("&amp;if((Q:Q&lt;&gt;"")*(Q:Q&lt;&gt;"Year"),Q:Q,"")&amp;if((Q:Q&lt;&gt;"")*(Q:Q&lt;&gt;"Year")*(M:M="Audit"),", ","")&amp;if(M:M="Audit","Audit","")&amp;If((M:M="Audit")*(N:N="Dropped"),", ","")&amp;if(N:N="Dropped","Dropped","")&amp;")",""))</f>
         <v>Formatted Course Title</v>
       </c>
-      <c r="T1" s="32" t="str">
-        <f t="array" ref="T1:T2">if(row(T:T)=1,"Include",(N:N="Enrolled")+((N:N="Dropped")*(countifs(Enrollment_Host_ID,A:A,Enrollment_CourseCode,G:G,Enrollment_Year,F:F,Enrollment_Term,Q:Q,Enrollment_Status,"Enrolled")=0)))</f>
-        <v>Include</v>
+      <c r="T1" s="34" t="b">
+        <f t="array" ref="T1:T2">if(row(T:T)=1,"Include",(N:N="Enrolled")+((N:N="Dropped")*(countifs(Enrollment_Host_ID,A:A,Enrollment_CourseCode,G:G,Enrollment_Year,F:F,Enrollment_Term,Q:Q,Enrollment_Status,"Enrolled")=0)))&gt;0</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="30">
+      <c r="R2" s="32">
         <v>0.0</v>
       </c>
-      <c r="S2" s="30" t="s">
+      <c r="S2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="30">
-        <v>0.0</v>
+      <c r="T2" s="32" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2097,362 +2105,360 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="35" t="s">
+      <c r="A1" s="36"/>
+      <c r="B1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38" t="str">
+      <c r="A2" s="39"/>
+      <c r="B2" s="40" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("if(A2&lt;&gt;"""",A2,REGEXEXTRACT(A1,""\[(.+)\]$""))"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="C2" s="38" t="str">
+      <c r="C2" s="40" t="str">
         <f t="array" ref="C2">INDEX('Advisor List'!E:E,match(B2,'Advisor List'!A:A,0),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="40" t="str">
+      <c r="B3" s="42" t="str">
         <f t="array" ref="B3:F3">IEH_GradYear-(6-COLUMN(B5:F5))</f>
         <v>#N/A</v>
       </c>
-      <c r="C3" s="40" t="e">
+      <c r="C3" s="42" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D3" s="41" t="e">
+      <c r="D3" s="43" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E3" s="41" t="e">
+      <c r="E3" s="43" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F3" s="42" t="e">
+      <c r="F3" s="44" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="46" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="43"/>
-      <c r="B5" s="45" t="str">
+      <c r="A5" s="45"/>
+      <c r="B5" s="47" t="str">
         <f t="array" ref="B5:F5">(B3:F3-1)&amp;" - "&amp;B3:F3</f>
         <v>#N/A</v>
       </c>
-      <c r="C5" s="45" t="e">
+      <c r="C5" s="47" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D5" s="45" t="e">
+      <c r="D5" s="47" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E5" s="45" t="e">
+      <c r="E5" s="47" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F5" s="45" t="e">
+      <c r="F5" s="47" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="47" t="str">
+      <c r="B6" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C6" s="47" t="str">
+      <c r="C6" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D6" s="47" t="str">
+      <c r="D6" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E6" s="47" t="str">
+      <c r="E6" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F6" s="47" t="str">
+      <c r="F6" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="47" t="str">
+      <c r="B7" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C7" s="47" t="str">
+      <c r="C7" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D7" s="47" t="str">
+      <c r="D7" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E7" s="47" t="str">
+      <c r="E7" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F7" s="47" t="str">
+      <c r="F7" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="47" t="str">
+      <c r="B8" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C8" s="47" t="str">
+      <c r="C8" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D8" s="47" t="str">
+      <c r="D8" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E8" s="47" t="str">
+      <c r="E8" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F8" s="47" t="str">
+      <c r="F8" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="47" t="str">
+      <c r="B9" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C9" s="47" t="str">
+      <c r="C9" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D9" s="47" t="str">
+      <c r="D9" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E9" s="47" t="str">
+      <c r="E9" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F9" s="47" t="str">
+      <c r="F9" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="47" t="str">
+      <c r="B10" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C10" s="47" t="str">
+      <c r="C10" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D10" s="47" t="str">
+      <c r="D10" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E10" s="47" t="str">
+      <c r="E10" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F10" s="47" t="str">
+      <c r="F10" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="47" t="str">
+      <c r="B11" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C11" s="47" t="str">
+      <c r="C11" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D11" s="47" t="str">
+      <c r="D11" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E11" s="47" t="str">
+      <c r="E11" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F11" s="47" t="str">
+      <c r="F11" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="47" t="str">
+      <c r="B12" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C12" s="47" t="str">
+      <c r="C12" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D12" s="47" t="str">
+      <c r="D12" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E12" s="47" t="str">
+      <c r="E12" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F12" s="47" t="str">
+      <c r="F12" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="47" t="str">
+      <c r="B13" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C13" s="47" t="str">
+      <c r="C13" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D13" s="47" t="str">
+      <c r="D13" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E13" s="47" t="str">
+      <c r="E13" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F13" s="47" t="str">
+      <c r="F13" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="47" t="str">
+      <c r="B14" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C14" s="47" t="str">
+      <c r="C14" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D14" s="47" t="str">
+      <c r="D14" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E14" s="47" t="str">
+      <c r="E14" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F14" s="47" t="str">
+      <c r="F14" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="47" t="str">
+      <c r="B15" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C15" s="47" t="str">
+      <c r="C15" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D15" s="47" t="str">
+      <c r="D15" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E15" s="47" t="str">
+      <c r="E15" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F15" s="47" t="str">
+      <c r="F15" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="47" t="str">
+      <c r="B16" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C16" s="47" t="str">
+      <c r="C16" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D16" s="47" t="str">
+      <c r="D16" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E16" s="47" t="str">
+      <c r="E16" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F16" s="47" t="str">
+      <c r="F16" s="49" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
@@ -2685,74 +2691,91 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="20.63"/>
-    <col customWidth="1" min="12" max="12" width="15.13"/>
+    <col customWidth="1" min="10" max="10" width="11.13"/>
+    <col customWidth="1" min="11" max="11" width="13.25"/>
+    <col customWidth="1" min="12" max="12" width="7.25"/>
+    <col customWidth="1" min="13" max="13" width="6.5"/>
+    <col customWidth="1" min="14" max="14" width="10.38"/>
+    <col customWidth="1" min="15" max="15" width="9.63"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="18" t="str">
+      <c r="D1" s="19" t="str">
         <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!B1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-2,false)),)</f>
         <v>Student Email</v>
       </c>
-      <c r="E1" s="18" t="str">
+      <c r="E1" s="19" t="str">
         <f t="array" ref="E1:E2">ifna(if(row(E:E)=1,'Advisor List'!C1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-2,false)),)</f>
         <v>Student First Name</v>
       </c>
-      <c r="F1" s="18" t="str">
+      <c r="F1" s="19" t="str">
         <f t="array" ref="F1:F2">ifna(if(row(F:F)=1,'Advisor List'!D1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-2,false)),)</f>
         <v>Student Last Name</v>
       </c>
-      <c r="G1" s="18" t="str">
+      <c r="G1" s="19" t="str">
         <f t="array" ref="G1:G2">ifna(if(row(G:G)=1,'Advisor List'!E1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-2,false)),)</f>
         <v>Grad Year</v>
       </c>
-      <c r="H1" s="19" t="str">
+      <c r="H1" s="20" t="str">
         <f t="array" ref="H1:H2">ifna(if(row(H:H)=1,'Student Folder Inventory'!B1,vlookup($A:$A,'Student Folder Inventory'!$A:$B,2,false)),)</f>
         <v>Student Folder ID</v>
       </c>
-      <c r="I1" s="20" t="str">
+      <c r="I1" s="21" t="str">
         <f t="array" ref="I1:I2">ifna(if(row(I:I)=1,'Advisor List'!F1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-3,false)),)</f>
         <v>Advisor Email</v>
       </c>
-      <c r="J1" s="18" t="str">
+      <c r="J1" s="19" t="str">
         <f t="array" ref="J1:J2">ifna(if(row(J:J)=1,'Advisor List'!G1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-3,false)),)</f>
         <v>Advisor First Name</v>
       </c>
-      <c r="K1" s="18" t="str">
+      <c r="K1" s="19" t="str">
         <f t="array" ref="K1:K2">ifna(if(row(K:K)=1,'Advisor List'!H1,vlookup($A:$A,'Advisor List'!$A:$H,COLUMN()-3,false)),)</f>
         <v>Advisor Last Name</v>
       </c>
-      <c r="L1" s="18" t="str">
+      <c r="L1" s="19" t="str">
         <f t="array" ref="L1:L2">ifna(if(row(L:L)=1,'Advisor Folder Inventory'!B1,vlookup($I:$I,'Advisor Folder Inventory'!$A:$B,2,false)),)</f>
         <v>Advisor Folder ID</v>
       </c>
-      <c r="M1" s="18" t="str">
+      <c r="M1" s="19" t="str">
         <f t="array" ref="M1:M2">ifna(if(row(M:M)=1,'Plans Form Folder Inventory'!B1,vlookup($G:$G,'Plans Form Folder Inventory'!$A:$B,2,false)),)</f>
         <v>Form Folder ID</v>
       </c>
+      <c r="N1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="23">
+        <v>3.0</v>
+      </c>
+      <c r="O2" s="23">
+        <v>6.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2782,30 +2805,30 @@
       <c r="C1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="25" t="str">
+      <c r="D1" s="26" t="str">
         <f t="array" ref="D1:D2">if($A:$A&lt;&gt;"",vlookup($A:$A,'Advisor List'!$A:$D,2,false),"")</f>
         <v>Student Email</v>
       </c>
-      <c r="E1" s="25" t="str">
+      <c r="E1" s="26" t="str">
         <f t="array" ref="E1:E2">if($A:$A&lt;&gt;"",vlookup($A:$A,'Advisor List'!$A:$D,3,false),"")</f>
         <v>Student First Name</v>
       </c>
-      <c r="F1" s="25" t="str">
+      <c r="F1" s="26" t="str">
         <f t="array" ref="F1:F2">if($A:$A&lt;&gt;"",vlookup($A:$A,'Advisor List'!$A:$D,4,false),"")</f>
         <v>Student Last Name</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="26" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2840,11 +2863,11 @@
       <c r="C1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="18" t="str">
+      <c r="D1" s="28" t="str">
         <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!G1,vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false)),)</f>
         <v>Advisor First Name</v>
       </c>
-      <c r="E1" s="18" t="str">
+      <c r="E1" s="28" t="str">
         <f t="array" ref="E1:E2">ifna(if(row(E:E)=1,'Advisor List'!H1,vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false)),)</f>
         <v>Advisor Last Name</v>
       </c>
@@ -2853,18 +2876,18 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="22" t="b">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2901,13 +2924,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="29" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2944,13 +2967,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="29" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2979,45 +3002,45 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="18" t="str">
+      <c r="I1" s="28" t="str">
         <f t="array" ref="I1:I2">if(row(I:I)=1,"Menu Option",D:D&amp;", "&amp;C:C&amp;" ’"&amp;(E:E-2000)&amp;" ["&amp;A:A&amp;"]")</f>
         <v>Menu Option</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
don’t import your parents!
Also renamed globals to be more identfiable, worked on #91 (need to figure out hwo structure generalizing the idea), added some more ignore files
</commit_message>
<xml_diff>
--- a/schema/sheets/Course Planning Data.xlsx
+++ b/schema/sheets/Course Planning Data.xlsx
@@ -74,7 +74,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">Last updated from "Advisor List" 8/8/2023, 11:28:01 AM</t>
+        <t xml:space="preserve">Last updated from "Advisor List" 8/11/2023, 7:12:09 AM</t>
       </text>
     </comment>
   </commentList>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
   <si>
     <t>Cell Color Legend</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Version</t>
+  </si>
+  <si>
+    <t>0.2.1</t>
   </si>
   <si>
     <t>Student Folder ID</t>
@@ -549,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -608,32 +611,38 @@
       <alignment vertical="center"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1024,11 +1033,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.5"/>
+    <col customWidth="1" min="1" max="1" width="36.63"/>
     <col customWidth="1" min="2" max="2" width="3.63"/>
   </cols>
   <sheetData>
@@ -1094,25 +1103,25 @@
         <v>26</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -1120,7 +1129,7 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="35"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -1147,51 +1156,51 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="32" t="s">
+      <c r="B1" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="29" t="str">
+      <c r="E1" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(F:F)=1,""Course Title"",iferror(index(REGEXEXTRACT(C:C,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
         <v>Course Title</v>
       </c>
-      <c r="G1" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="29" t="s">
+      <c r="G1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="H1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="29" t="str">
+      <c r="I1" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula(if(row(E:E)=1,""Formatted Description"",trim(REGEXREPLACE(SUBSTITUTE(substitute(E:E,""&lt;br /&gt;"",char(10)),""&amp;#160;"","" ""),""&lt;\/\w+&gt;|&lt;\w+.*?&gt;"",""""))))"),"Formatted Description")</f>
         <v>Formatted Description</v>
       </c>
-      <c r="K1" s="29" t="str">
+      <c r="K1" s="31" t="str">
         <f t="array" ref="K1:K2">if(row(K:K)=1,"Available",vlookup(A:A,'Available Courses'!A2:F$3,6,false))</f>
         <v>Available</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34" t="str">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36" t="str">
         <f t="array" ref="G2">SWITCH(right(C2,3),"(F)","Fall","(W)","Winter","(S)","Spring",)</f>
         <v/>
       </c>
@@ -1239,38 +1248,38 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="C1" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="D1" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="F1" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="G1" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="H1" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="I1" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="J1" s="31" t="s">
         <v>68</v>
+      </c>
+      <c r="K1" s="31" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2">
@@ -2070,105 +2079,105 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="B1" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="32" t="s">
+      <c r="E1" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="G1" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="H1" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="I1" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="J1" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="K1" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="L1" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="M1" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="29" t="str">
+      <c r="N1" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(Enrollment_BaseTitle)=1,""Base Title"",if(Enrollment_CourseCode=5741,""Advanced Physics: Electricity and Magnetism"",iferror(index(REGEXEXTRACT(Enrollment_TitleWithTerm,""^(.+)( \([FWSY]\))$""),0,1),Enrollment_TitleWithTerm))))"),"Base Title")</f>
         <v>Base Title</v>
       </c>
-      <c r="P1" s="29" t="str">
+      <c r="P1" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(Enrollment_ParentheticalNote)=1,""Parenthetical Note"",ifna(REGEXEXTRACT(Enrollment_BaseTitle,""\((.+)\)""),)))"),"Parenthetical Note")</f>
         <v>Parenthetical Note</v>
       </c>
-      <c r="Q1" s="29" t="str">
+      <c r="Q1" s="31" t="str">
         <f t="array" ref="Q1:Q2">if(row(Enrollment_Department)=1,"Department",ifna(if(Enrollment_DepartmentList="History and Social Science | Philosophy and Religious Studies","History and Social Science",Enrollment_DepartmentList)))</f>
         <v>Department</v>
       </c>
-      <c r="R1" s="29" t="str">
+      <c r="R1" s="31" t="str">
         <f t="array" ref="R1:R2">if(row(Enrollment_Term)=1,"Term",if(Enrollment_CourseCode=5741,"Fall, Winter",SWITCH(right(Enrollment_TitleWithTerm,3),"(F)","Fall","(W)","Winter","(S)","Spring","(Y)", "Year","Year")))</f>
         <v>Term</v>
       </c>
-      <c r="S1" s="29" t="str">
+      <c r="S1" s="31" t="str">
         <f t="array" ref="S1:S2">if(row(Enrollment_Order)=1,"Order",switch(Enrollment_TermName,"Fall Term",1,"Winter Term",2,"Spring Term",3,0)-if(Enrollment_Status="Dropped",0.5,0))</f>
         <v>Order</v>
       </c>
-      <c r="T1" s="29" t="str">
+      <c r="T1" s="31" t="str">
         <f t="array" ref="T1:T2">if(row(Enrollment_Title)=1,"Formatted Course Title",if(Enrollment_ParentheticalNote&lt;&gt;"",left(Enrollment_BaseTitle, len(Enrollment_BaseTitle)-1),Enrollment_BaseTitle)&amp;if((Enrollment_Type="Audit")+(Enrollment_Status="Dropped")+((Enrollment_Term&lt;&gt;"Year")*(Enrollment_Term&lt;&gt;"")),if(Enrollment_ParentheticalNote&lt;&gt;"",", "," (")&amp;if((Enrollment_Term&lt;&gt;"")*(Enrollment_Term&lt;&gt;"Year"),Enrollment_Term,"")&amp;if((Enrollment_Term&lt;&gt;"")*(Enrollment_Term&lt;&gt;"Year")*(Enrollment_Type="Audit"),", ","")&amp;if(Enrollment_Type="Audit","Audit","")&amp;If((Enrollment_Type="Audit")*(Enrollment_Status="Dropped"),", ","")&amp;if(Enrollment_Status="Dropped","Dropped","")&amp;")",if(Enrollment_ParentheticalNote&lt;&gt;"",")","")))</f>
         <v>Formatted Course Title</v>
       </c>
-      <c r="U1" s="36" t="str">
+      <c r="U1" s="38" t="str">
         <f t="array" ref="U1:U2">if(row(Enrollment_Include)=1,"Include",((Enrollment_Status="Enrolled")+((Enrollment_Status="Dropped")*(countifs(Enrollment_Host_ID,Enrollment_Host_ID,Enrollment_CourseCode,Enrollment_CourseCode,Enrollment_Year,Enrollment_Year,Enrollment_Term,Enrollment_Term,Enrollment_Status,"Enrolled")=0)))&gt;0)</f>
         <v>Include</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="S2" s="34">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="S2" s="36">
         <v>0.0</v>
       </c>
-      <c r="T2" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="34" t="b">
+      <c r="T2" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="36" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2192,365 +2201,365 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39" t="s">
+      <c r="A1" s="40"/>
+      <c r="B1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="39" t="s">
+      <c r="C1" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="D1" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42" t="str">
+      <c r="A2" s="43"/>
+      <c r="B2" s="44" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("if(A2&lt;&gt;"""",A2,REGEXEXTRACT(A1,""\[(.+)\]$""))"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="C2" s="42" t="str">
+      <c r="C2" s="44" t="str">
         <f t="array" ref="C2">join(" ",INDEX('Advisor List'!C:D,match(B2,'Advisor List'!A:A,0),0))</f>
         <v>#N/A</v>
       </c>
-      <c r="D2" s="42" t="str">
+      <c r="D2" s="44" t="str">
         <f t="array" ref="D2">INDEX('Advisor List'!E:E,match(B2,'Advisor List'!A:A,0),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3">
-      <c r="A3" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="44" t="str">
+      <c r="A3" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="46" t="str">
         <f t="array" ref="B3:F3">IEH_GradYear-(6-COLUMN(B5:F5))</f>
         <v>#N/A</v>
       </c>
-      <c r="C3" s="44" t="e">
+      <c r="C3" s="46" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D3" s="45" t="e">
+      <c r="D3" s="47" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E3" s="45" t="e">
+      <c r="E3" s="47" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F3" s="46" t="e">
+      <c r="F3" s="48" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="48" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="C4" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="D4" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="E4" s="50" t="s">
         <v>90</v>
       </c>
+      <c r="F4" s="50" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="47"/>
-      <c r="B5" s="49" t="str">
+      <c r="A5" s="49"/>
+      <c r="B5" s="51" t="str">
         <f t="array" ref="B5:F5">(B3:F3-1)&amp;" - "&amp;B3:F3</f>
         <v>#N/A</v>
       </c>
-      <c r="C5" s="49" t="e">
+      <c r="C5" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D5" s="49" t="e">
+      <c r="D5" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E5" s="49" t="e">
+      <c r="E5" s="51" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F5" s="49" t="e">
+      <c r="F5" s="51" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="51" t="str">
+      <c r="A6" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C6" s="51" t="str">
+      <c r="C6" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D6" s="51" t="str">
+      <c r="D6" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E6" s="51" t="str">
+      <c r="E6" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F6" s="51" t="str">
+      <c r="F6" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="51" t="str">
+      <c r="A7" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C7" s="51" t="str">
+      <c r="C7" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D7" s="51" t="str">
+      <c r="D7" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E7" s="51" t="str">
+      <c r="E7" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F7" s="51" t="str">
+      <c r="F7" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="51" t="str">
+      <c r="A8" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C8" s="51" t="str">
+      <c r="C8" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D8" s="51" t="str">
+      <c r="D8" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E8" s="51" t="str">
+      <c r="E8" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F8" s="51" t="str">
+      <c r="F8" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="51" t="str">
+      <c r="A9" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C9" s="51" t="str">
+      <c r="C9" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D9" s="51" t="str">
+      <c r="D9" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E9" s="51" t="str">
+      <c r="E9" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F9" s="51" t="str">
+      <c r="F9" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="51" t="str">
+      <c r="A10" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C10" s="51" t="str">
+      <c r="C10" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D10" s="51" t="str">
+      <c r="D10" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E10" s="51" t="str">
+      <c r="E10" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F10" s="51" t="str">
+      <c r="F10" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="51" t="str">
+      <c r="A11" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C11" s="51" t="str">
+      <c r="C11" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D11" s="51" t="str">
+      <c r="D11" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E11" s="51" t="str">
+      <c r="E11" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F11" s="51" t="str">
+      <c r="F11" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="51" t="str">
+      <c r="A12" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C12" s="51" t="str">
+      <c r="C12" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D12" s="51" t="str">
+      <c r="D12" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E12" s="51" t="str">
+      <c r="E12" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F12" s="51" t="str">
+      <c r="F12" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="51" t="str">
+      <c r="A13" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C13" s="51" t="str">
+      <c r="C13" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D13" s="51" t="str">
+      <c r="D13" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E13" s="51" t="str">
+      <c r="E13" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F13" s="51" t="str">
+      <c r="F13" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="51" t="str">
+      <c r="A14" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C14" s="51" t="str">
+      <c r="C14" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D14" s="51" t="str">
+      <c r="D14" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E14" s="51" t="str">
+      <c r="E14" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F14" s="51" t="str">
+      <c r="F14" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="51" t="str">
+      <c r="A15" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C15" s="51" t="str">
+      <c r="C15" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D15" s="51" t="str">
+      <c r="D15" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E15" s="51" t="str">
+      <c r="E15" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F15" s="51" t="str">
+      <c r="F15" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="51" t="str">
+      <c r="A16" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C16" s="51" t="str">
+      <c r="C16" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D16" s="51" t="str">
+      <c r="D16" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E16" s="51" t="str">
+      <c r="E16" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F16" s="51" t="str">
+      <c r="F16" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
@@ -2793,14 +2802,21 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.63"/>
+    <col customWidth="1" min="1" max="1" width="7.0"/>
+    <col customWidth="1" min="2" max="2" width="7.38"/>
+    <col customWidth="1" min="3" max="3" width="7.0"/>
+    <col customWidth="1" min="4" max="4" width="9.5"/>
+    <col customWidth="1" min="7" max="7" width="4.88"/>
+    <col customWidth="1" min="8" max="9" width="7.13"/>
     <col customWidth="1" min="10" max="10" width="11.13"/>
     <col customWidth="1" min="11" max="11" width="13.25"/>
-    <col customWidth="1" min="12" max="12" width="7.25"/>
-    <col customWidth="1" min="13" max="13" width="6.5"/>
+    <col customWidth="1" min="12" max="12" width="7.38"/>
+    <col customWidth="1" min="13" max="13" width="6.13"/>
     <col customWidth="1" min="14" max="14" width="10.38"/>
-    <col customWidth="1" min="15" max="17" width="9.63"/>
-    <col customWidth="1" min="18" max="19" width="11.13"/>
+    <col customWidth="1" min="15" max="15" width="9.63"/>
+    <col customWidth="1" min="16" max="17" width="7.25"/>
+    <col customWidth="1" min="18" max="18" width="11.13"/>
+    <col customWidth="1" min="19" max="19" width="7.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2903,9 +2919,8 @@
       <c r="R2" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="S2" s="23" t="str">
-        <f>"0.2.0"</f>
-        <v>0.2.0</v>
+      <c r="S2" s="23" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2933,36 +2948,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="28" t="str">
+      <c r="C1" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="29" t="str">
         <f t="array" ref="D1:D2">if($A:$A&lt;&gt;"",ifna(vlookup($A:$A,'Advisor List'!$A:$D,2,false),vlookup($A:$A,'Advisor List (Previous Year)'!$A:$D,2,false)),"")</f>
         <v>Student Email</v>
       </c>
-      <c r="E1" s="28" t="str">
+      <c r="E1" s="29" t="str">
         <f t="array" ref="E1:E2">if($A:$A&lt;&gt;"",ifna(vlookup($A:$A,'Advisor List'!$A:$D,3,false),vlookup($A:$A,'Advisor List (Previous Year)'!$A:$D,3,false)),"")</f>
         <v>Student First Name</v>
       </c>
-      <c r="F1" s="28" t="str">
+      <c r="F1" s="29" t="str">
         <f t="array" ref="F1:F2">if($A:$A&lt;&gt;"",ifna(vlookup($A:$A,'Advisor List'!$A:$D,4,false),vlookup($A:$A,'Advisor List (Previous Year)'!$A:$D,4,false)),"")</f>
         <v>Student Last Name</v>
       </c>
-      <c r="G1" s="20" t="str">
+      <c r="G1" s="30" t="str">
         <f t="array" ref="G1:G2">if(row(G:G)=1,"Inactive",isna(vlookup(A:A,'Advisor List'!A:A,1)))</f>
         <v>Inactive</v>
       </c>
-      <c r="H1" s="20" t="str">
+      <c r="H1" s="30" t="str">
         <f t="array" ref="H1:H2">if(row(H:H)=1,"New Advisor",iferror(if((G:G=false)*(xlookup(A:A,'Advisor List'!A:A,'Advisor List'!F:F)&lt;&gt;xlookup(A:A,'Advisor List (Previous Year)'!A:A,'Advisor List (Previous Year)'!F:F))=1,true,false),false))</f>
         <v>New Advisor</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="28" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2971,13 +2986,13 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G2" s="27" t="b">
         <v>1</v>
@@ -3012,35 +3027,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="29" t="str">
-        <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!G1,vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false)),)</f>
+        <v>37</v>
+      </c>
+      <c r="D1" s="31" t="str">
+        <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!G1,ifna(vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false),vlookup($A:$A,'Advisor List (Previous Year)'!$F:$H,COLUMN()-2,false))),)</f>
         <v>Advisor First Name</v>
       </c>
-      <c r="E1" s="29" t="str">
-        <f t="array" ref="E1:E2">ifna(if(row(E:E)=1,'Advisor List'!H1,vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false)),)</f>
+      <c r="E1" s="31" t="str">
+        <f t="array" ref="E1:E2">ifna(if(row(E:E)=1,'Advisor List'!H1,ifna(vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false),vlookup($A:$A,'Advisor List (Previous Year)'!$F:$H,COLUMN()-2,false))),)</f>
         <v>Advisor Last Name</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="30" t="s">
         <v>40</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>41</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -3071,24 +3086,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="30" t="s">
         <v>40</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3114,24 +3129,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="30" t="s">
         <v>40</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3159,46 +3174,46 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="32" t="s">
+      <c r="B1" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="D1" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="32" t="s">
+      <c r="E1" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="F1" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="29" t="str">
+      <c r="H1" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="31" t="str">
         <f t="array" ref="I1:I2">if(row(I:I)=1,"Menu Option",D:D&amp;", "&amp;C:C&amp;" ’"&amp;(E:E-2000)&amp;" ["&amp;A:A&amp;"]")</f>
         <v>Menu Option</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34" t="s">
-        <v>52</v>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="36" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add to inventory sooner
Close #85

Tag plans that are in the inventory but not yet complete as incomplete.
</commit_message>
<xml_diff>
--- a/schema/sheets/Course Planning Data.xlsx
+++ b/schema/sheets/Course Planning Data.xlsx
@@ -74,7 +74,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">Last updated from "Advisor List" 8/11/2023, 7:12:09 AM</t>
+        <t xml:space="preserve">Last updated from "Advisor List" 8/15/2023, 1:02:33 PM</t>
       </text>
     </comment>
   </commentList>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
   <si>
     <t>Cell Color Legend</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Version</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
   </si>
   <si>
     <t>0.2.1</t>
@@ -1103,25 +1106,25 @@
         <v>26</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
@@ -1160,7 +1163,7 @@
         <v>21</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>22</v>
@@ -1169,20 +1172,20 @@
         <v>23</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F1" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(F:F)=1,""Course Title"",iferror(index(REGEXEXTRACT(C:C,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
         <v>Course Title</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J1" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula(if(row(E:E)=1,""Formatted Description"",trim(REGEXREPLACE(SUBSTITUTE(substitute(E:E,""&lt;br /&gt;"",char(10)),""&amp;#160;"","" ""),""&lt;\/\w+&gt;|&lt;\w+.*?&gt;"",""""))))"),"Formatted Description")</f>
@@ -1249,37 +1252,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J1" s="31" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2">
@@ -2080,46 +2083,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="34" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N1" s="34" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O1" s="31" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(Enrollment_BaseTitle)=1,""Base Title"",if(Enrollment_CourseCode=5741,""Advanced Physics: Electricity and Magnetism"",iferror(index(REGEXEXTRACT(Enrollment_TitleWithTerm,""^(.+)( \([FWSY]\))$""),0,1),Enrollment_TitleWithTerm))))"),"Base Title")</f>
@@ -2169,13 +2172,13 @@
       <c r="P2" s="36"/>
       <c r="Q2" s="36"/>
       <c r="R2" s="36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="S2" s="36">
         <v>0.0</v>
       </c>
       <c r="T2" s="36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="U2" s="36" t="b">
         <v>0</v>
@@ -2206,10 +2209,10 @@
         <v>26</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="42"/>
       <c r="F1" s="42"/>
@@ -2233,7 +2236,7 @@
     </row>
     <row r="3">
       <c r="A3" s="45" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B3" s="46" t="str">
         <f t="array" ref="B3:F3">IEH_GradYear-(6-COLUMN(B5:F5))</f>
@@ -2255,19 +2258,19 @@
     <row r="4">
       <c r="A4" s="49"/>
       <c r="B4" s="50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5">
@@ -2291,7 +2294,7 @@
     </row>
     <row r="6">
       <c r="A6" s="52" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B6" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
@@ -2316,7 +2319,7 @@
     </row>
     <row r="7">
       <c r="A7" s="52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
@@ -2341,7 +2344,7 @@
     </row>
     <row r="8">
       <c r="A8" s="52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
@@ -2366,7 +2369,7 @@
     </row>
     <row r="9">
       <c r="A9" s="52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B9" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
@@ -2391,7 +2394,7 @@
     </row>
     <row r="10">
       <c r="A10" s="52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B10" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
@@ -2416,7 +2419,7 @@
     </row>
     <row r="11">
       <c r="A11" s="52" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
@@ -2441,7 +2444,7 @@
     </row>
     <row r="12">
       <c r="A12" s="52" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B12" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
@@ -2466,7 +2469,7 @@
     </row>
     <row r="13">
       <c r="A13" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
@@ -2491,7 +2494,7 @@
     </row>
     <row r="14">
       <c r="A14" s="52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B14" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
@@ -2516,7 +2519,7 @@
     </row>
     <row r="15">
       <c r="A15" s="52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B15" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
@@ -2541,7 +2544,7 @@
     </row>
     <row r="16">
       <c r="A16" s="52" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B16" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
@@ -2667,11 +2670,14 @@
     </row>
   </sheetData>
   <dataValidations>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B10">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(B10))), AND(ISNUMBER(B10), LEFT(CELL("format", B10))="D"))</formula1>
+    </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B2">
       <formula1>2.0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B10">
-      <formula1>OR(NOT(ISERROR(DATEVALUE(B10))), AND(ISNUMBER(B10), LEFT(CELL("format", B10))="D"))</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B1">
+      <formula1>1.0</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B9">
       <formula1>IFERROR(ISURL(B9), true)</formula1>
@@ -2681,9 +2687,6 @@
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B7:B8">
       <formula1>IFERROR(ISEMAIL(B7), true)</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B1">
-      <formula1>1.0</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -2816,7 +2819,7 @@
     <col customWidth="1" min="15" max="15" width="9.63"/>
     <col customWidth="1" min="16" max="17" width="7.25"/>
     <col customWidth="1" min="18" max="18" width="11.13"/>
-    <col customWidth="1" min="19" max="19" width="7.0"/>
+    <col customWidth="1" min="19" max="20" width="7.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2876,7 +2879,7 @@
         <v>8</v>
       </c>
       <c r="P1" s="20" t="str">
-        <f t="array" ref="P1:P2">if(row(P:P)=1,"Inactive",isna(vlookup(A:A,'Advisor List'!A:A,1)))</f>
+        <f t="array" ref="P1:P2">if(row(P:P)=1,"Inactive", isna(vlookup(A:A,'Advisor List'!A:A,1,false)))</f>
         <v>Inactive</v>
       </c>
       <c r="Q1" s="20" t="str">
@@ -2888,6 +2891,9 @@
       </c>
       <c r="S1" s="19" t="s">
         <v>30</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -2920,7 +2926,10 @@
         <v>0</v>
       </c>
       <c r="S2" s="23" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="T2" s="23" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2952,10 +2961,10 @@
         <v>26</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="29" t="str">
         <f t="array" ref="D1:D2">if($A:$A&lt;&gt;"",ifna(vlookup($A:$A,'Advisor List'!$A:$D,2,false),vlookup($A:$A,'Advisor List (Previous Year)'!$A:$D,2,false)),"")</f>
@@ -2970,7 +2979,7 @@
         <v>Student Last Name</v>
       </c>
       <c r="G1" s="30" t="str">
-        <f t="array" ref="G1:G2">if(row(G:G)=1,"Inactive",isna(vlookup(A:A,'Advisor List'!A:A,1)))</f>
+        <f t="array" ref="G1:G2">if(row(G:G)=1,"Inactive",isna(vlookup(A:A,'Advisor List'!A:A,1,false)))</f>
         <v>Inactive</v>
       </c>
       <c r="H1" s="30" t="str">
@@ -2986,13 +2995,13 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G2" s="27" t="b">
         <v>1</v>
@@ -3027,13 +3036,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" s="31" t="str">
         <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!G1,ifna(vlookup($A:$A,'Advisor List'!$F:$H,COLUMN()-2,false),vlookup($A:$A,'Advisor List (Previous Year)'!$F:$H,COLUMN()-2,false))),)</f>
@@ -3044,18 +3053,18 @@
         <v>Advisor Last Name</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -3086,24 +3095,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3129,24 +3138,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3171,6 +3180,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="9" max="9" width="32.63"/>
+    <col customWidth="1" min="10" max="11" width="11.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3178,29 +3188,37 @@
         <v>26</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I1" s="31" t="str">
         <f t="array" ref="I1:I2">if(row(I:I)=1,"Menu Option",D:D&amp;", "&amp;C:C&amp;" ’"&amp;(E:E-2000)&amp;" ["&amp;A:A&amp;"]")</f>
         <v>Menu Option</v>
+      </c>
+      <c r="J1" s="31" t="str">
+        <f t="array" ref="J1:J2">if(row(J:J)=1,"New Student",isna(vlookup(A:A,'Advisor List (Previous Year)'!A:A,1,false)))</f>
+        <v>New Student</v>
+      </c>
+      <c r="K1" s="31" t="str">
+        <f t="array" ref="K1:K2">if(row(K:K)=1,"New Advisor",xlookup(A:A,'Advisor List (Previous Year)'!A:A,'Advisor List (Previous Year)'!F:F)&lt;&gt;F:F)</f>
+        <v>New Advisor</v>
       </c>
     </row>
     <row r="2">
@@ -3213,7 +3231,13 @@
       <c r="G2" s="35"/>
       <c r="H2" s="35"/>
       <c r="I2" s="36" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="J2" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="36" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix broken formatted course descriptions
</commit_message>
<xml_diff>
--- a/schema/sheets/Course Planning Data.xlsx
+++ b/schema/sheets/Course Planning Data.xlsx
@@ -79,17 +79,17 @@
     <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">'Student Folder Inventory'!$A$1:$J$2</definedName>
     <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">'Advisor Folder Inventory'!$A$1:$F$2</definedName>
     <definedName hidden="1" localSheetId="15" name="_xlnm._FilterDatabase">'Student Enrollments'!$A$1:$AB$2</definedName>
-    <definedName hidden="1" localSheetId="4" name="Z_19212B59_ADC0_4C7C_B33B_E4180A0A832B_.wvu.FilterData">'Course Plan Inventory'!$A$1:$S$2</definedName>
-    <definedName hidden="1" localSheetId="5" name="Z_19212B59_ADC0_4C7C_B33B_E4180A0A832B_.wvu.FilterData">'Student Folder Inventory'!$A$1:$J$2</definedName>
-    <definedName hidden="1" localSheetId="6" name="Z_19212B59_ADC0_4C7C_B33B_E4180A0A832B_.wvu.FilterData">'Advisor Folder Inventory'!$A$1:$F$2</definedName>
-    <definedName hidden="1" localSheetId="9" name="Z_19212B59_ADC0_4C7C_B33B_E4180A0A832B_.wvu.FilterData">'Student List'!$A$1:$N$2</definedName>
-    <definedName hidden="1" localSheetId="4" name="Z_673A4590_BC65_4BC5_8F96_361B74C7351F_.wvu.FilterData">'Course Plan Inventory'!$A$1:$S$2</definedName>
-    <definedName hidden="1" localSheetId="9" name="Z_673A4590_BC65_4BC5_8F96_361B74C7351F_.wvu.FilterData">'Student List'!$A$1:$N$2</definedName>
+    <definedName hidden="1" localSheetId="4" name="Z_0D1BABFC_5A64_4F6D_B3B2_985CB56A84C6_.wvu.FilterData">'Course Plan Inventory'!$A$1:$S$2</definedName>
+    <definedName hidden="1" localSheetId="5" name="Z_0D1BABFC_5A64_4F6D_B3B2_985CB56A84C6_.wvu.FilterData">'Student Folder Inventory'!$A$1:$J$2</definedName>
+    <definedName hidden="1" localSheetId="6" name="Z_0D1BABFC_5A64_4F6D_B3B2_985CB56A84C6_.wvu.FilterData">'Advisor Folder Inventory'!$A$1:$F$2</definedName>
+    <definedName hidden="1" localSheetId="9" name="Z_0D1BABFC_5A64_4F6D_B3B2_985CB56A84C6_.wvu.FilterData">'Student List'!$A$1:$N$2</definedName>
+    <definedName hidden="1" localSheetId="4" name="Z_A955676D_EF55_4F9A_978F_61A99DC86708_.wvu.FilterData">'Course Plan Inventory'!$A$1:$S$2</definedName>
+    <definedName hidden="1" localSheetId="9" name="Z_A955676D_EF55_4F9A_978F_61A99DC86708_.wvu.FilterData">'Student List'!$A$1:$N$2</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{673A4590-BC65-4BC5-8F96-361B74C7351F}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{19212B59-ADC0-4C7C-B33B-E4180A0A832B}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A955676D-EF55-4F9A-978F-61A99DC86708}" name="Filter 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0D1BABFC-5A64-4F6D-B3B2-985CB56A84C6}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -147,7 +147,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">Last updated from "Course List" 4/4/2024, 12:05:47 PM</t>
+        <t xml:space="preserve">Last updated from "Course List" 4/10/2024, 8:49:52 AM</t>
       </text>
     </comment>
   </commentList>
@@ -3752,7 +3752,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{673A4590-BC65-4BC5-8F96-361B74C7351F}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{A955676D-EF55-4F9A-978F-61A99DC86708}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$N$2">
         <filterColumn colId="13">
           <filters>
@@ -3761,7 +3761,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{19212B59-ADC0-4C7C-B33B-E4180A0A832B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0D1BABFC-5A64-4F6D-B3B2-985CB56A84C6}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$N$2">
         <filterColumn colId="13">
           <filters>
@@ -8038,7 +8038,7 @@
         <v>853</v>
       </c>
       <c r="K1" s="22" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula(if(row(F:F)=1,""Formatted Description"",trim(REGEXREPLACE(SUBSTITUTE(substitute(F:F,""&lt;br /&gt;"",char(10)),""&amp;#160;"","" ""),""&lt;\/\w+&gt;|&lt;\w+.*?&gt;"",""""))))"),"Formatted Description")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula(if(row(F:F)=1,""Formatted Description"",trim(REGEXREPLACE(SUBSTITUTE(substitute(E:E,""&lt;br /&gt;"",char(10)),""&amp;#160;"","" ""),""&lt;\/\w+&gt;|&lt;\w+.*?&gt;"",""""))))"),"Formatted Description")</f>
         <v>Formatted Description</v>
       </c>
       <c r="L1" s="22" t="str">
@@ -8077,8 +8077,8 @@
         <v/>
       </c>
       <c r="K2" s="37" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"FALSE")</f>
-        <v>FALSE</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
+        <v/>
       </c>
       <c r="L2" s="37" t="e">
         <v>#N/A</v>
@@ -9508,8 +9508,9 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="8.88"/>
     <col customWidth="1" min="2" max="2" width="11.38"/>
-    <col customWidth="1" min="3" max="3" width="53.75"/>
+    <col customWidth="1" min="3" max="3" width="37.38"/>
     <col customWidth="1" min="4" max="4" width="27.88"/>
+    <col customWidth="1" min="5" max="5" width="47.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9833,7 +9834,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{673A4590-BC65-4BC5-8F96-361B74C7351F}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{A955676D-EF55-4F9A-978F-61A99DC86708}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$S$2">
         <filterColumn colId="14">
           <filters>
@@ -9842,7 +9843,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{19212B59-ADC0-4C7C-B33B-E4180A0A832B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0D1BABFC-5A64-4F6D-B3B2-985CB56A84C6}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$S$2">
         <filterColumn colId="6">
           <filters/>
@@ -9954,7 +9955,7 @@
     </sortState>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{19212B59-ADC0-4C7C-B33B-E4180A0A832B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0D1BABFC-5A64-4F6D-B3B2-985CB56A84C6}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$J$2"/>
     </customSheetView>
   </customSheetViews>
@@ -10038,7 +10039,7 @@
     </sortState>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{19212B59-ADC0-4C7C-B33B-E4180A0A832B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0D1BABFC-5A64-4F6D-B3B2-985CB56A84C6}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$F$2">
         <filterColumn colId="5">
           <filters>

</xml_diff>

<commit_message>
refactor!: remove annual roll-over and supporting data structures
</commit_message>
<xml_diff>
--- a/schema/sheets/Course Planning Data.xlsx
+++ b/schema/sheets/Course Planning Data.xlsx
@@ -40,16 +40,18 @@
     <definedName name="Student_First_Name">'Student List'!$C:$C</definedName>
     <definedName name="Grad_Year">'Student List'!$E:$E</definedName>
     <definedName name="Param_CollegeCounselingOffice">Parameters!$B$10</definedName>
-    <definedName name="StudentList_StudentEmail">'Student List'!$B:$B</definedName>
+    <definedName name="Student_Email">'Student List'!$B:$B</definedName>
     <definedName name="Enrollment_TitleWithTerm">'Student Enrollments'!$H:$H</definedName>
     <definedName name="IEH_NumericalYears">'Individual Enrollment History'!$B$3:$F$3</definedName>
     <definedName name="IEH_Departments">'Individual Enrollment History'!$A$6:$A$16</definedName>
     <definedName name="Label_StudentFirstName">'Student List'!$C$1</definedName>
+    <definedName name="Student_Grad_Year">'Student List'!$E:$E</definedName>
     <definedName name="Enrollment_ParentheticalNote">'Student Enrollments'!$W:$W</definedName>
     <definedName name="Param_CoursePlanTemplate">Parameters!$B$11</definedName>
     <definedName name="Enrollment_TermName">'Student Enrollments'!$K:$K</definedName>
     <definedName name="Course_Title">'Course List'!$C$2</definedName>
     <definedName name="Enrollment_TitleWithoutTerm">'Student Enrollments'!$T:$T</definedName>
+    <definedName name="Student_Menu_Listing">'Student List'!$H:$H</definedName>
     <definedName name="Faculty_Host_ID">'Faculty List'!$A:$A</definedName>
     <definedName name="Param_AcademicOffice">Parameters!$B$8</definedName>
     <definedName name="Faculty_Email">'Faculty List'!$D:$D</definedName>
@@ -62,17 +64,17 @@
     <definedName name="Course_Available">'Course List'!$L$2</definedName>
     <definedName name="Advisor_Email">'Advisor List'!$G:$G</definedName>
     <definedName name="CrossRegistered_Department">'Cross-registered Courses'!$C$3</definedName>
+    <definedName name="Student_Inactive">'Student List'!$G:$G</definedName>
     <definedName name="Enrollment_Order">'Student Enrollments'!$V:$V</definedName>
     <definedName name="Student_Last_Name">'Student List'!$D:$D</definedName>
     <definedName name="Enrollment_Dropped">'Student Enrollments'!$O:$O</definedName>
     <definedName name="Course_Department">'Course List'!$N$2</definedName>
     <definedName name="Param_StudiesCommittee">Parameters!$B$9</definedName>
     <definedName name="Clean_AvailableCourses">'Available Courses'!$A$3</definedName>
-    <definedName name="RollOver_CoursePlanPermissions">#REF!</definedName>
+    <definedName name="Advisor_Most_Likely_Advisor">'Advisor List'!$K:$K</definedName>
     <definedName name="Enrollment_BaseTitle">'Student Enrollments'!$U:$U</definedName>
     <definedName name="Param_AdvisorFolderNameFormat">Parameters!$B$6</definedName>
     <definedName name="Course_CrossRegistered">'Course List'!$M$2</definedName>
-    <definedName name="Param_RollOverAcademicYear">Parameters!$B$12</definedName>
     <definedName name="Enrollment_CreditsAttempted">'Student Enrollments'!$R:$R</definedName>
     <definedName name="Advisor_Host_ID">'Advisor List'!$A:$A</definedName>
     <definedName name="CrossRegistered_CourseCode">'Cross-registered Courses'!$A$3</definedName>
@@ -84,9 +86,7 @@
     <definedName name="Grad_Year_Label">'Student List'!$E$1</definedName>
     <definedName name="Student_Host_ID_Label">'Student List'!$A$1</definedName>
     <definedName name="Enrollment_Enrolled">'Student Enrollments'!$N:$N</definedName>
-    <definedName name="Enrollment_Type">#REF!</definedName>
     <definedName name="Param_NumOptionsPerDepartment">Parameters!$B$1</definedName>
-    <definedName name="RollOver_StudentFolderPermissions">#REF!</definedName>
     <definedName name="Course_Plan_Host_ID">'Course Plan Inventory'!$A:$A</definedName>
     <definedName name="Enrollment_Annotation">'Student Enrollments'!$W:$Z</definedName>
     <definedName name="Faculty_First_Name_Label">'Faculty List'!$B$1</definedName>
@@ -94,23 +94,24 @@
     <definedName name="Enrollment_Term">'Student Enrollments'!$X:$X</definedName>
     <definedName name="Clean_IEH">'Individual Enrollment History'!$A$1:$A$2</definedName>
     <definedName name="Current_Advisor">'Advisor List'!$J:$J</definedName>
-    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'Available Courses'!$A$1:$F$3</definedName>
+    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'Available Courses'!$A$2:$F$3</definedName>
     <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">'Cross-registered Courses'!$A$2:$P$3</definedName>
+    <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">'Course Plan Inventory'!$A$1:$R$2</definedName>
     <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">'Student Folder Inventory'!$A$1:$K$2</definedName>
     <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">'Advisor Folder Inventory'!$A$1:$F$2</definedName>
     <definedName hidden="1" localSheetId="11" name="_xlnm._FilterDatabase">'Advisor List'!$A$1:$J$2</definedName>
     <definedName hidden="1" localSheetId="14" name="_xlnm._FilterDatabase">'Student Enrollments'!$A$1:$AB$2</definedName>
-    <definedName hidden="1" localSheetId="4" name="Z_6AD4D4A6_ED0D_40E6_8DEF_5D96ED6B85A3_.wvu.FilterData">'Course Plan Inventory'!$A$1:$S$2</definedName>
-    <definedName hidden="1" localSheetId="9" name="Z_6AD4D4A6_ED0D_40E6_8DEF_5D96ED6B85A3_.wvu.FilterData">'Student List'!$A$1:$F$2</definedName>
-    <definedName hidden="1" localSheetId="4" name="Z_3FBFD739_53C5_42AA_9D25_C0C9F903DD50_.wvu.FilterData">'Course Plan Inventory'!$A$1:$S$2</definedName>
-    <definedName hidden="1" localSheetId="5" name="Z_3FBFD739_53C5_42AA_9D25_C0C9F903DD50_.wvu.FilterData">'Student Folder Inventory'!$A$1:$J$2</definedName>
-    <definedName hidden="1" localSheetId="6" name="Z_3FBFD739_53C5_42AA_9D25_C0C9F903DD50_.wvu.FilterData">'Advisor Folder Inventory'!$A$1:$F$2</definedName>
-    <definedName hidden="1" localSheetId="9" name="Z_3FBFD739_53C5_42AA_9D25_C0C9F903DD50_.wvu.FilterData">'Student List'!$A$1:$F$2</definedName>
+    <definedName hidden="1" localSheetId="4" name="Z_8A0215D2_B727_4E45_BA43_9D0FF4AE1D0C_.wvu.FilterData">'Course Plan Inventory'!$A$1:$R$2</definedName>
+    <definedName hidden="1" localSheetId="9" name="Z_8A0215D2_B727_4E45_BA43_9D0FF4AE1D0C_.wvu.FilterData">'Student List'!$A$1:$F$2</definedName>
+    <definedName hidden="1" localSheetId="4" name="Z_C8DFF587_8138_47F6_882F_E53E2855F909_.wvu.FilterData">'Course Plan Inventory'!$A$1:$R$2</definedName>
+    <definedName hidden="1" localSheetId="5" name="Z_C8DFF587_8138_47F6_882F_E53E2855F909_.wvu.FilterData">'Student Folder Inventory'!$A$1:$J$2</definedName>
+    <definedName hidden="1" localSheetId="6" name="Z_C8DFF587_8138_47F6_882F_E53E2855F909_.wvu.FilterData">'Advisor Folder Inventory'!$A$1:$F$2</definedName>
+    <definedName hidden="1" localSheetId="9" name="Z_C8DFF587_8138_47F6_882F_E53E2855F909_.wvu.FilterData">'Student List'!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{6AD4D4A6-ED0D-40E6-8DEF-5D96ED6B85A3}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3FBFD739-53C5-42AA-9D25-C0C9F903DD50}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{8A0215D2-B727-4E45-BA43-9D0FF4AE1D0C}" name="Filter 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C8DFF587-8138-47F6-882F-E53E2855F909}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -123,7 +124,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">Last updated from "Student List" 9/19/2025, 2:51:14 PM</t>
+        <t xml:space="preserve">Last updated from "Student List" 10/21/2025, 9:42:30 AM</t>
       </text>
     </comment>
   </commentList>
@@ -138,7 +139,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">Last updated from "Faculty List" 8/15/2025, 9:16:37 AM</t>
+        <t xml:space="preserve">Last updated from "Faculty List" 10/21/2025, 9:42:15 AM</t>
       </text>
     </comment>
   </commentList>
@@ -153,7 +154,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">Last updated from "Advisor List" 9/9/2025, 1:24:22 PM</t>
+        <t xml:space="preserve">Last updated from "Advisor List" 10/21/2025, 9:41:43 AM</t>
       </text>
     </comment>
   </commentList>
@@ -168,7 +169,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">Last updated from "Course List" 8/15/2025, 9:02:22 AM</t>
+        <t xml:space="preserve">Last updated from "Course List" 10/21/2025, 9:41:08 AM</t>
       </text>
     </comment>
   </commentList>
@@ -183,7 +184,7 @@
   <commentList>
     <comment authorId="0" ref="A1">
       <text>
-        <t xml:space="preserve">Last updated from "Student Enrollments" 8/15/2025, 8:59:00 AM</t>
+        <t xml:space="preserve">Last updated from "Student Enrollments" 10/21/2025, 9:40:08 AM</t>
       </text>
     </comment>
   </commentList>
@@ -253,7 +254,7 @@
     <t>Academic Office</t>
   </si>
   <si>
-    <t>email@example.com</t>
+    <t>cp-ao@groton.org</t>
   </si>
   <si>
     <t>Studies Committee</t>
@@ -265,12 +266,6 @@
     <t>Course Plan Template</t>
   </si>
   <si>
-    <t>Roll-over Academic Year</t>
-  </si>
-  <si>
-    <t>2024-08-21T15:24:52.401Z</t>
-  </si>
-  <si>
     <t>Course ID</t>
   </si>
   <si>
@@ -310,6 +305,9 @@
     <t>Incomplete</t>
   </si>
   <si>
+    <t>rholmes@groton.org</t>
+  </si>
+  <si>
     <t>Student Folder ID</t>
   </si>
   <si>
@@ -362,6 +360,9 @@
   </si>
   <si>
     <t>Grad Year</t>
+  </si>
+  <si>
+    <t>,  []</t>
   </si>
   <si>
     <t>Preferred or First Name</t>
@@ -503,9 +504,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy h:mm:ss"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy h:mm:ss"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -699,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="66">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -734,9 +734,6 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -790,9 +787,6 @@
     <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -804,9 +798,6 @@
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
@@ -829,7 +820,7 @@
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1339,43 +1330,58 @@
     <col customWidth="1" min="3" max="3" width="11.25"/>
     <col customWidth="1" min="4" max="4" width="17.88"/>
     <col customWidth="1" min="5" max="5" width="4.88"/>
-    <col customWidth="1" min="6" max="6" width="6.13"/>
+    <col customWidth="1" min="6" max="7" width="6.13"/>
+    <col customWidth="1" min="8" max="8" width="34.25"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="43" t="s">
+      <c r="A1" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="30" t="str">
+      <c r="F1" s="29" t="str">
         <f t="array" ref="F1:F2">if(row(F:F)=1,"Has Plan",not(isna(vlookup(A:A,'Course Plan Inventory'!A:A,1,false))))</f>
         <v>Has Plan</v>
       </c>
+      <c r="G1" s="29" t="str">
+        <f t="array" ref="G1:G2">if(row(G:G)=1,"Inactive",not(E:E&gt;(year(today())+if(month(today())&gt;6,1,0))))</f>
+        <v>Inactive</v>
+      </c>
+      <c r="H1" s="29" t="str">
+        <f t="array" ref="H1:H2">if(row(H:H)=1,"Menu Listing",D:D&amp;", "&amp;C:C&amp;" ["&amp;A:A&amp;"]")</f>
+        <v>Menu Listing</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="26" t="b">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="25" t="b">
         <v>0</v>
+      </c>
+      <c r="G2" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6AD4D4A6-ED0D-40E6-8DEF-5D96ED6B85A3}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{8A0215D2-B727-4E45-BA43-9D0FF4AE1D0C}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$F$2">
         <filterColumn colId="5">
           <filters>
@@ -1384,7 +1390,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{3FBFD739-53C5-42AA-9D25-C0C9F903DD50}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{C8DFF587-8138-47F6-882F-E53E2855F909}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$F$2">
         <filterColumn colId="5">
           <filters>
@@ -1394,12 +1400,12 @@
       </autoFilter>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="F2">
+  <conditionalFormatting sqref="F2:H2">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"FALSE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
+  <conditionalFormatting sqref="F2:H2">
     <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"TRUE"</formula>
     </cfRule>
@@ -1423,24 +1429,26 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="45" t="s">
+      <c r="A1" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="42" t="s">
         <v>59</v>
       </c>
+      <c r="E1" s="42"/>
     </row>
     <row r="2">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>
@@ -1475,72 +1483,72 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="43" t="s">
+      <c r="A1" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="43" t="s">
+      <c r="G1" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="30" t="str">
+      <c r="J1" s="29" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("byrow({A:A,F:F},lambda(enrollment,if(index(enrollment,1,1)=$A$1,""Current Advisor"",index(enrollment,1,2)=max(filter({A:A,F:F},A:A=index(enrollment,1,1))))))"),"Current Advisor")</f>
         <v>Current Advisor</v>
       </c>
-      <c r="K1" s="30" t="str">
+      <c r="K1" s="29" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("BYROW(A:I,lambda(data,if(index(data,1,1)=$A$1,""Most Likely Advisor"",max(filter(F:F,A:A=index(data,1,1)))=index(data,1,6))))"),"Most Likely Advisor")</f>
         <v>Most Likely Advisor</v>
       </c>
-      <c r="L1" s="30" t="str">
-        <f t="array" ref="L1:L2">byrow(A:I,lambda(data,if(index(data,1,1)=$A$1,"Advisor on Course Plan",xlookup(index(data,1,1),'Course Plan Inventory'!A:A,'Course Plan Inventory'!Q:Q)=index(data,1,7))))</f>
+      <c r="L1" s="29" t="str">
+        <f t="array" ref="L1:L2">byrow(A:I,lambda(data,if(index(data,1,1)=$A$1,"Advisor on Course Plan",xlookup(index(data,1,1),'Course Plan Inventory'!A:A,'Course Plan Inventory'!P:P)=index(data,1,7))))</f>
         <v>Advisor on Course Plan</v>
       </c>
-      <c r="M1" s="30" t="str">
+      <c r="M1" s="29" t="str">
         <f t="array" ref="M1:M2">xlookup(G:G,'Advisor Folder Inventory'!A:A,'Advisor Folder Inventory'!C:C)</f>
         <v>Advisor Folder URL</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="26" t="b">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="25" t="b">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),TRUE)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="26" t="b">
+      <c r="K2" s="25" t="b">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),TRUE)</f>
         <v>1</v>
       </c>
-      <c r="L2" s="26" t="e">
+      <c r="L2" s="25" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M2" s="26" t="e">
+      <c r="M2" s="25" t="e">
         <v>#N/A</v>
       </c>
     </row>
@@ -1587,85 +1595,85 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="22" t="str">
+      <c r="G1" s="21" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(G:G)=1,""Course Title"",iferror(index(REGEXEXTRACT(C:C,""^(.+) \([FWSY]\)""),0,0))))"),"Course Title")</f>
         <v>Course Title</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="22" t="str">
+      <c r="K1" s="21" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula(if(row(F:F)=1,""Formatted Description"",trim(REGEXREPLACE(SUBSTITUTE(substitute(E:E,""&lt;br /&gt;"",char(10)),""&amp;#160;"","" ""),""&lt;\/\w+&gt;|&lt;\w+.*?&gt;"",""""))))"),"Formatted Description")</f>
         <v>Formatted Description</v>
       </c>
-      <c r="L1" s="22" t="str">
+      <c r="L1" s="21" t="str">
         <f t="array" ref="L1:L2">if(row(L:L)=1,"Available",if(F:F,false,vlookup(A:A,'Available Courses'!A2:F$3,6,false)))</f>
         <v>Available</v>
       </c>
-      <c r="M1" s="22" t="str">
+      <c r="M1" s="21" t="str">
         <f t="array" ref="M1:M2">if(row(M:M)=1,"Cross-registered",countif($B$2:$B2,B:B)&lt;&gt;countifs($B$2:$B2,B:B,$D$2:$D2,D:D))</f>
         <v>Cross-registered</v>
       </c>
-      <c r="N1" s="22" t="str">
+      <c r="N1" s="21" t="str">
         <f t="array" ref="N1:N2">byrow({B:B,D:D,M:M},lambda(row,if(index(row,1,1)="Course Code","Display Department",if(index(row,1,3),if(index(CrossRegistered_Department,match(index(row,1,1),CrossRegistered_CourseCode,0),0)&lt;&gt;"",index(CrossRegistered_Department,match(index(row,1,1),CrossRegistered_CourseCode,0),0),index(row,1,2)),INDEX(row,1,2)))))</f>
         <v>Display Department</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26" t="str">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="str">
         <f t="array" ref="H2">SWITCH(right(C2,3),"(F)","Fall","(W)","Winter","(S)","Spring",)</f>
         <v/>
       </c>
-      <c r="I2" s="38">
+      <c r="I2" s="35">
         <f t="array" ref="I2">switch(H2,"Fall",1,"Winter",2,"Spring",3,0)</f>
         <v>0</v>
       </c>
-      <c r="J2" s="38" t="str">
+      <c r="J2" s="35" t="str">
         <f t="array" ref="J2">if(H2&lt;&gt;"",if(countif(Course_Title,G2&amp;" (Y)"),,G2&amp;" ("&amp;H2&amp;")"),G2)</f>
         <v/>
       </c>
-      <c r="K2" s="38" t="str">
+      <c r="K2" s="35" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="L2" s="38" t="e">
+      <c r="L2" s="35" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M2" s="38" t="b">
+      <c r="M2" s="35" t="b">
         <v>0</v>
       </c>
-      <c r="N2" s="38"/>
+      <c r="N2" s="35"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:N2">
@@ -1695,223 +1703,730 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="46" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=A1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="A2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=A1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="B2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=B1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="B2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=B1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="C2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=C1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="C2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=C1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="D2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=D1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="D2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=D1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="E2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=E1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="E2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=E1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="F2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=F1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="F2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=F1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="G2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=G1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="G2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=G1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="H2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=H1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="H2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=H1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="I2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=I1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="I2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=I1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="J2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=J1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="J2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=J1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="K2" s="50" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J5,Course_Department=K1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
+      <c r="K2" s="47" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("arrayformula({unique(index(sort(filter('Course List'!$G$2:$J44,Course_Department=K1,Course_Available),3,true,1,true),,4));"""";""[Elective]"";""[Tutorial]""})"),"#N/A")</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="50" t="str">
+      <c r="A3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="B3" s="50" t="str">
+      <c r="B3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="C3" s="50" t="str">
+      <c r="C3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="D3" s="50" t="str">
+      <c r="D3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="E3" s="50" t="str">
+      <c r="E3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="F3" s="50" t="str">
+      <c r="F3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="G3" s="50" t="str">
+      <c r="G3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="H3" s="50" t="str">
+      <c r="H3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="I3" s="50" t="str">
+      <c r="I3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="J3" s="50" t="str">
+      <c r="J3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
-      <c r="K3" s="50" t="str">
+      <c r="K3" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"")</f>
         <v/>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="50" t="str">
+      <c r="A4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="B4" s="50" t="str">
+      <c r="B4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="C4" s="50" t="str">
+      <c r="C4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="D4" s="50" t="str">
+      <c r="D4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="E4" s="50" t="str">
+      <c r="E4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="F4" s="50" t="str">
+      <c r="F4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="G4" s="50" t="str">
+      <c r="G4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="H4" s="50" t="str">
+      <c r="H4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="I4" s="50" t="str">
+      <c r="I4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="J4" s="50" t="str">
+      <c r="J4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
-      <c r="K4" s="50" t="str">
+      <c r="K4" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Elective]")</f>
         <v>[Elective]</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="50" t="str">
+      <c r="A5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="B5" s="50" t="str">
+      <c r="B5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="C5" s="50" t="str">
+      <c r="C5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="D5" s="50" t="str">
+      <c r="D5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="E5" s="50" t="str">
+      <c r="E5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="F5" s="50" t="str">
+      <c r="F5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="G5" s="50" t="str">
+      <c r="G5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="H5" s="50" t="str">
+      <c r="H5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="I5" s="50" t="str">
+      <c r="I5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="J5" s="50" t="str">
+      <c r="J5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
-      <c r="K5" s="50" t="str">
+      <c r="K5" s="47" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"[Tutorial]")</f>
         <v>[Tutorial]</v>
       </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="47"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="47"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="47"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="47"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="47"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="47"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="47"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="47"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="47"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="47"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="47"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="47"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="47"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="47"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="47"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="47"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="47"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="47"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="47"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="47"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="47"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="47"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="47"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="47"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="47"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="47"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="47"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="47"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="47"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="47"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="47"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="47"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="47"/>
+      <c r="B44" s="47"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="47"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1942,138 +2457,138 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="52" t="s">
+      <c r="A1" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="52" t="s">
+      <c r="D1" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="52" t="s">
+      <c r="I1" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="52" t="s">
+      <c r="M1" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="O1" s="52" t="s">
+      <c r="O1" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="T1" s="53" t="str">
+      <c r="T1" s="50" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(Enrollment_TitleWithoutTerm)=1,""Title without Term"",if(Enrollment_CourseCode=5741,""Advanced Physics: Electricity and Magnetism"",iferror(index(REGEXEXTRACT(Enrollment_TitleWithTerm,""^(.+)( \([FWSY]\)\.*)$""),0,1),Enrollment_TitleWi"&amp;"thTerm))))"),"Title without Term")</f>
         <v>Title without Term</v>
       </c>
-      <c r="U1" s="53" t="str">
+      <c r="U1" s="50" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(U:U)=1,""Base Title"",REGEXEXTRACT(Enrollment_TitleWithoutTerm,""([^(]+)\s?\(?.*\)?"")))"),"Base Title")</f>
         <v>Base Title</v>
       </c>
-      <c r="V1" s="53" t="str">
+      <c r="V1" s="50" t="str">
         <f t="array" ref="V1:V2">if(row(Enrollment_Order)=1,"Order",switch(Enrollment_TermName,"Fall",1,"Winter",2,"Spring",3,0)-if(Enrollment_Dropped,0.5,0))</f>
         <v>Order</v>
       </c>
-      <c r="W1" s="53" t="str">
+      <c r="W1" s="50" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(Enrollment_ParentheticalNote)=1,""Parenthetical Note"",ifna(REGEXEXTRACT(Enrollment_TitleWithoutTerm,""\((.+)\)""),)))"),"Parenthetical Note")</f>
         <v>Parenthetical Note</v>
       </c>
-      <c r="X1" s="53" t="str">
+      <c r="X1" s="50" t="str">
         <f t="array" ref="X1:X2">if(row(Enrollment_Term)=1,"Term",if(Enrollment_CourseCode=5741,"Fall, Winter",SWITCH(right(Enrollment_TitleWithTerm,3),"(F)","Fall","(W)","Winter","(S)","Spring","(Y)", "","")))</f>
         <v>Term</v>
       </c>
-      <c r="Y1" s="53" t="str">
+      <c r="Y1" s="50" t="str">
         <f t="array" ref="Y1:Y2">if(row(Y:Y)=1,"Audit",if((Enrollment_CreditsAttempted="")*not(Enrollment_Dropped)*(today()&gt;Q:Q),"audit",))</f>
         <v>Audit</v>
       </c>
-      <c r="Z1" s="53" t="str">
+      <c r="Z1" s="50" t="str">
         <f t="array" ref="Z1:Z2">if(row(Z:Z)=1,"Dropped",if(Enrollment_Dropped*not(Enrollment_ChangedSections),"dropped",))</f>
         <v>Dropped</v>
       </c>
-      <c r="AA1" s="53" t="str">
+      <c r="AA1" s="50" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ARRAYFORMULA(if(row(AA:AA)=1,""Enrollment Title"",substitute(Enrollment_BaseTitle&amp;"" (""&amp;substitute(trim(transpose(query(transpose(W:Z),,ROWS(AA:AA)))),"" "","", "")&amp;"")"","" ()"","""")))"),"#REF!")</f>
         <v>#REF!</v>
       </c>
-      <c r="AB1" s="54" t="str">
+      <c r="AB1" s="51" t="str">
         <f t="array" ref="AB1:AB2">if(row(Enrollment_Include)=1,"Include",NOT(vlookup(Enrollment_CourseCode,'Course List'!B:M,12,false)*((countifs('Course List'!B:B,Enrollment_CourseCode,'Course List'!N:N,Enrollment_Department)=0)))*(not(Enrollment_Dropped)+Enrollment_Dropped*not(Enrollment_ChangedSections))&gt;0)</f>
         <v>Include</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26" t="str">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="V2" s="26">
+      <c r="V2" s="25">
         <v>0.0</v>
       </c>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26" t="s">
+      <c r="W2" s="25"/>
+      <c r="X2" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="Y2" s="26" t="s">
+      <c r="Y2" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26" t="e">
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25" t="e">
         <v>#N/A</v>
       </c>
     </row>
@@ -2099,365 +2614,365 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="55"/>
-      <c r="B1" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="56" t="s">
+      <c r="A1" s="52"/>
+      <c r="B1" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
     </row>
     <row r="2">
-      <c r="A2" s="58"/>
-      <c r="B2" s="59" t="str">
+      <c r="A2" s="55"/>
+      <c r="B2" s="56" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("if(A2&lt;&gt;"""",A2,REGEXEXTRACT(A1,""\[(.+)\]$""))"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="C2" s="59" t="str">
+      <c r="C2" s="56" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("join("" "",INDEX('Student List'!C:D,match(B2,'Student List'!A:A,0),0))"),"#N/A")</f>
         <v>#N/A</v>
       </c>
-      <c r="D2" s="59" t="str">
+      <c r="D2" s="56" t="str">
         <f t="array" ref="D2">INDEX('Student List'!E:E,match(B2,'Student List'!A:A,0),0)</f>
         <v>#N/A</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="61" t="str">
+      <c r="B3" s="58" t="str">
         <f t="array" ref="B3:F3">IEH_GradYear-(6-COLUMN(B5:F5))</f>
         <v>#N/A</v>
       </c>
-      <c r="C3" s="61" t="e">
+      <c r="C3" s="58" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D3" s="62" t="e">
+      <c r="D3" s="59" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E3" s="62" t="e">
+      <c r="E3" s="59" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F3" s="63" t="e">
+      <c r="F3" s="60" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="64"/>
-      <c r="B4" s="65" t="s">
+      <c r="A4" s="61"/>
+      <c r="B4" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="E4" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="65" t="s">
+      <c r="F4" s="62" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="64"/>
-      <c r="B5" s="66" t="str">
+      <c r="A5" s="61"/>
+      <c r="B5" s="63" t="str">
         <f t="array" ref="B5:F5">(B3:F3-1)&amp;" - "&amp;B3:F3</f>
         <v>#N/A</v>
       </c>
-      <c r="C5" s="66" t="e">
+      <c r="C5" s="63" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D5" s="66" t="e">
+      <c r="D5" s="63" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E5" s="66" t="e">
+      <c r="E5" s="63" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F5" s="66" t="e">
+      <c r="F5" s="63" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="68" t="str">
+      <c r="B6" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C6" s="68" t="str">
+      <c r="C6" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D6" s="68" t="str">
+      <c r="D6" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E6" s="68" t="str">
+      <c r="E6" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F6" s="68" t="str">
+      <c r="F6" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A6),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="68" t="str">
+      <c r="B7" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C7" s="68" t="str">
+      <c r="C7" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D7" s="68" t="str">
+      <c r="D7" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E7" s="68" t="str">
+      <c r="E7" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F7" s="68" t="str">
+      <c r="F7" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A7),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="68" t="str">
+      <c r="B8" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C8" s="68" t="str">
+      <c r="C8" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D8" s="68" t="str">
+      <c r="D8" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E8" s="68" t="str">
+      <c r="E8" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F8" s="68" t="str">
+      <c r="F8" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A8),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="68" t="str">
+      <c r="B9" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C9" s="68" t="str">
+      <c r="C9" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D9" s="68" t="str">
+      <c r="D9" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E9" s="68" t="str">
+      <c r="E9" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F9" s="68" t="str">
+      <c r="F9" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A9),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="68" t="str">
+      <c r="B10" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C10" s="68" t="str">
+      <c r="C10" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D10" s="68" t="str">
+      <c r="D10" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E10" s="68" t="str">
+      <c r="E10" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F10" s="68" t="str">
+      <c r="F10" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A10),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="68" t="str">
+      <c r="B11" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C11" s="68" t="str">
+      <c r="C11" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D11" s="68" t="str">
+      <c r="D11" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E11" s="68" t="str">
+      <c r="E11" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F11" s="68" t="str">
+      <c r="F11" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A11),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="68" t="str">
+      <c r="B12" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C12" s="68" t="str">
+      <c r="C12" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D12" s="68" t="str">
+      <c r="D12" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E12" s="68" t="str">
+      <c r="E12" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F12" s="68" t="str">
+      <c r="F12" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A12),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="68" t="str">
+      <c r="B13" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C13" s="68" t="str">
+      <c r="C13" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D13" s="68" t="str">
+      <c r="D13" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E13" s="68" t="str">
+      <c r="E13" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F13" s="68" t="str">
+      <c r="F13" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A13),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="67" t="s">
+      <c r="A14" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="68" t="str">
+      <c r="B14" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C14" s="68" t="str">
+      <c r="C14" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D14" s="68" t="str">
+      <c r="D14" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E14" s="68" t="str">
+      <c r="E14" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F14" s="68" t="str">
+      <c r="F14" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A14),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="68" t="str">
+      <c r="B15" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C15" s="68" t="str">
+      <c r="C15" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D15" s="68" t="str">
+      <c r="D15" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E15" s="68" t="str">
+      <c r="E15" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F15" s="68" t="str">
+      <c r="F15" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A15),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="68" t="str">
+      <c r="B16" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=B$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="C16" s="68" t="str">
+      <c r="C16" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=C$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="D16" s="68" t="str">
+      <c r="D16" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=D$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="E16" s="68" t="str">
+      <c r="E16" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=E$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
-      <c r="F16" s="68" t="str">
+      <c r="F16" s="65" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IFNA(JOIN(CHAR(10),UNIQUE(INDEX(SORT(FILTER({Enrollment_Title, Enrollment_Order},Enrollment_Include,Enrollment_Host_ID=IEH_HostID,Enrollment_Year=F$5,Enrollment_Department=$A16),2,true,1,true),,1))),)"),"")</f>
         <v/>
       </c>
@@ -2465,7 +2980,7 @@
   </sheetData>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A1">
-      <formula1>#REF!</formula1>
+      <formula1>'Student List'!$H$2:$H16</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -2571,14 +3086,6 @@
       </c>
       <c r="B11" s="11"/>
     </row>
-    <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B11">
@@ -2592,9 +3099,6 @@
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B2">
       <formula1>2.0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="B12">
-      <formula1>OR(NOT(ISERROR(DATEVALUE(B12))), AND(ISNUMBER(B12), LEFT(CELL("format", B12))="D"))</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B8:B10">
       <formula1>IFERROR(ISEMAIL(B8), true)</formula1>
@@ -2625,44 +3129,44 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="str">
+      <c r="A1" s="12" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ifna(""Missing: ""&amp;join("", "",filter(Course_Title,isna(Course_Available))),""All courses synced from Blackbaud are shown in this list. Scan the list for red/yellow highlighted duplicates if necessary."")"),"Missing: ")</f>
         <v>Missing: </v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="15" t="str">
+      <c r="A2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="14" t="str">
         <f t="array" ref="B2:E3">vlookup($A2:$A3,{'Course List'!$A:$D,'Course List'!$K:$K},column(B:E),false)</f>
         <v>Course Code</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="F2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18" t="e">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C3" s="18" t="e">
+      <c r="C3" s="17" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D3" s="18" t="e">
+      <c r="D3" s="17" t="e">
         <v>#N/A</v>
       </c>
-      <c r="E3" s="18" t="e">
+      <c r="E3" s="17" t="e">
         <v>#N/A</v>
       </c>
       <c r="F3" s="7" t="b">
@@ -2670,7 +3174,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$F$3"/>
+  <autoFilter ref="$A$2:$F$3"/>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
@@ -2718,71 +3222,71 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="19" t="str">
+      <c r="A1" s="18" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("ifna(""Missing: ""&amp;join("", "",sort(unique(filter(Course_Code,isna(Course_Department))))),""All detected cross-registered courses are shown in this list."")"),"All detected cross-registered courses are shown in this list.")</f>
         <v>All detected cross-registered courses are shown in this list.</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2">
-      <c r="A2" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="22" t="str">
+      <c r="A2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="21" t="str">
         <f t="array" ref="B2:B3">if(row(B2:B3)=2,"Course Title",vlookup(A2:A3,'Course List'!B:C,2,false))</f>
         <v>Course Title</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="24" t="str">
+      <c r="C2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="23" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("byrow(A2:A3,lambda(code,if(code=""Course Code"",""Registered Departments"",if(code&lt;&gt;"""",transpose(sort(unique(filter('Course List'!D:D,'Course List'!B:B=code)))),))))"),"Registered Departments")</f>
         <v>Registered Departments</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
     </row>
     <row r="3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26" t="e">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25" t="e">
         <v>#N/A</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$2:$P$3">
@@ -2826,141 +3330,140 @@
     <col customWidth="1" min="4" max="4" width="10.13"/>
     <col customWidth="1" min="7" max="7" width="7.63"/>
     <col customWidth="1" min="8" max="8" width="11.25"/>
-    <col customWidth="1" min="9" max="9" width="9.88"/>
-    <col customWidth="1" min="10" max="10" width="12.25"/>
-    <col customWidth="1" min="11" max="11" width="13.25"/>
-    <col customWidth="1" min="12" max="12" width="10.63"/>
-    <col customWidth="1" min="13" max="13" width="11.13"/>
-    <col customWidth="1" min="14" max="14" width="13.25"/>
-    <col customWidth="1" min="15" max="15" width="9.63"/>
-    <col customWidth="1" min="16" max="17" width="9.88"/>
-    <col customWidth="1" min="18" max="18" width="9.63"/>
-    <col customWidth="1" min="19" max="19" width="12.38"/>
+    <col customWidth="1" min="9" max="9" width="12.25"/>
+    <col customWidth="1" min="10" max="10" width="13.25"/>
+    <col customWidth="1" min="11" max="11" width="10.63"/>
+    <col customWidth="1" min="12" max="12" width="11.13"/>
+    <col customWidth="1" min="13" max="13" width="13.25"/>
+    <col customWidth="1" min="14" max="14" width="9.63"/>
+    <col customWidth="1" min="15" max="16" width="9.88"/>
+    <col customWidth="1" min="17" max="17" width="9.63"/>
+    <col customWidth="1" min="18" max="19" width="12.38"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="30" t="str">
-        <f t="array" ref="D1:D2">ifna(if(row(E:E)=1,Label_StudentEmail,ifna(xlookup(Course_Plan_Host_ID,Student_Host_ID,StudentList_StudentEmail),)),"")</f>
+      <c r="D1" s="29" t="str">
+        <f t="array" ref="D1:D2">ifna(if(row(E:E)=1,Label_StudentEmail,ifna(xlookup(Course_Plan_Host_ID,Student_Host_ID,Student_Email),)),"")</f>
         <v>Student Email</v>
       </c>
-      <c r="E1" s="30" t="str">
+      <c r="E1" s="29" t="str">
         <f t="array" ref="E1:E2">ifna(if(row(F:F)=1,Label_StudentFirstName,ifna(xlookup(Course_Plan_Host_ID,Student_Host_ID,Student_First_Name),)),"")</f>
         <v>Student First Name</v>
       </c>
-      <c r="F1" s="30" t="str">
+      <c r="F1" s="29" t="str">
         <f t="array" ref="F1:F2">ifna(if(row(G:G)=1,Student_Last_Name_Label,ifna(xlookup(Course_Plan_Host_ID,Student_Host_ID,Student_Last_Name),)),"")</f>
         <v>Student Last Name</v>
       </c>
-      <c r="G1" s="30" t="str">
+      <c r="G1" s="29" t="str">
         <f t="array" ref="G1:G2">ifna(if(row(H:H)=1,Grad_Year_Label,ifna(xlookup(Course_Plan_Host_ID,Student_Host_ID,Grad_Year),)),"")</f>
         <v>Grad Year</v>
       </c>
-      <c r="H1" s="31" t="str">
+      <c r="H1" s="30" t="str">
         <f t="array" ref="H1:H2">ifna(if(row(H:H)=1,'Student Folder Inventory'!B1,vlookup($A:$A,'Student Folder Inventory'!$A:$B,2,false)),)</f>
         <v>Student Folder ID</v>
       </c>
-      <c r="I1" s="32" t="str">
-        <f t="array" ref="I1:I2">if(row(J:J)=1,'Advisor List'!G1,ifna(xlookup(A:A,'Advisor List'!A:A,'Advisor List'!G:G),))</f>
+      <c r="I1" s="29" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("byrow(A:A,lambda(host_id,if(host_id=$A$1,""Advisor Email"",ifna(filter(Advisor_Email,Advisor_Host_ID=host_id,Advisor_Most_Likely_Advisor),))))"),"Advisor Email")</f>
         <v>Advisor Email</v>
       </c>
-      <c r="J1" s="30" t="str">
-        <f t="array" ref="J1:J2">if(row(J:J)=1,'Advisor List'!G1,ifna(xlookup(A:A,'Advisor List'!A:A,'Advisor List'!G:G),))</f>
-        <v>Advisor Email</v>
-      </c>
-      <c r="K1" s="30" t="str">
-        <f t="array" ref="K1:K2">ifna(if(row(K:K)=1,'Advisor List'!I1,ifna(vlookup($A:$A,'Advisor List'!$A:$I,COLUMN()-3,false),)),)</f>
+      <c r="J1" s="29" t="str">
+        <f t="array" ref="J1:J2">ifna(if(row(J:J)=1,'Advisor List'!I1,ifna(vlookup($A:$A,'Advisor List'!$A:$I,COLUMN()-3,false),)),)</f>
         <v>Advisor Last Name</v>
       </c>
-      <c r="L1" s="30" t="str">
-        <f t="array" ref="L1:L2">ifna(if(row(L:L)=1,'Advisor Folder Inventory'!B1,vlookup($I:$I,'Advisor Folder Inventory'!$A:$B,2,false)),)</f>
+      <c r="K1" s="29" t="str">
+        <f t="array" ref="K1:K2">ifna(if(row(K:K)=1,'Advisor Folder Inventory'!B1,vlookup(J:J,'Advisor Folder Inventory'!$A:$B,2,false)),)</f>
         <v>Advisor Folder ID</v>
       </c>
-      <c r="M1" s="30" t="str">
-        <f t="array" ref="M1:M2">ifna(if(row(M:M)=1,'Plans Form Folder Inventory'!B1,vlookup($G:$G,'Plans Form Folder Inventory'!$A:$B,2,false)),)</f>
+      <c r="L1" s="29" t="str">
+        <f t="array" ref="L1:L2">ifna(if(row(L:L)=1,'Plans Form Folder Inventory'!B1,vlookup($G:$G,'Plans Form Folder Inventory'!$A:$B,2,false)),)</f>
         <v>Form Folder ID</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="M1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="30" t="str">
-        <f t="array" ref="O1:O2">if(row(O:O)=1,"Inactive", isna(vlookup(A:A,'Student List'!A:A,1,false)))</f>
+      <c r="N1" s="29" t="str">
+        <f t="array" ref="N1:N2">if(row(N:N)=1,"Inactive",IFNA(not(xlookup(A:A,'Student List'!A:A,not('Student List'!G:G))),true))</f>
         <v>Inactive</v>
       </c>
-      <c r="P1" s="30" t="str">
-        <f t="array" ref="P1:P2">if(row(P:P)=1,"New Advisor",J:J&lt;&gt;Q:Q)</f>
+      <c r="O1" s="29" t="str">
+        <f t="array" ref="O1:O2">if(row(O:O)=1,"New Advisor",I:I&lt;&gt;P:P)</f>
         <v>New Advisor</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="P1" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="S1" s="28"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="N2" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="P2" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34" t="b">
-        <v>0</v>
-      </c>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
     </row>
   </sheetData>
+  <autoFilter ref="$A$1:$R$2"/>
   <customSheetViews>
-    <customSheetView guid="{6AD4D4A6-ED0D-40E6-8DEF-5D96ED6B85A3}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$A$1:$S$2">
-        <filterColumn colId="14">
+    <customSheetView guid="{8A0215D2-B727-4E45-BA43-9D0FF4AE1D0C}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$A$1:$R$2">
+        <filterColumn colId="13">
           <filters>
             <filter val="TRUE"/>
           </filters>
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{3FBFD739-53C5-42AA-9D25-C0C9F903DD50}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$A$1:$S$2">
+    <customSheetView guid="{C8DFF587-8138-47F6-882F-E53E2855F909}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$A$1:$R$2">
         <filterColumn colId="6">
           <filters/>
         </filterColumn>
       </autoFilter>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="O2:Q2">
+  <conditionalFormatting sqref="N2:P2">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"FALSE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:Q2">
+  <conditionalFormatting sqref="N2:P2">
     <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"TRUE"</formula>
     </cfRule>
@@ -2995,63 +3498,63 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="29" t="s">
+      <c r="A1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="40" t="str">
+      <c r="D1" s="37" t="str">
         <f t="array" ref="D1:D2">ifna(if(row(E:E)=1,'Student List'!B1,ifna(xlookup($A:$A,'Student List'!$A:$A,'Student List'!B:B),)),"")</f>
         <v>Student Email</v>
       </c>
-      <c r="E1" s="40" t="str">
+      <c r="E1" s="37" t="str">
         <f t="array" ref="E1:E2">ifna(if(row(F:F)=1,'Student List'!C1,ifna(xlookup($A:$A,'Student List'!$A:$A,'Student List'!C:C),)),"")</f>
         <v>Student First Name</v>
       </c>
-      <c r="F1" s="40" t="str">
+      <c r="F1" s="37" t="str">
         <f t="array" ref="F1:F2">ifna(if(row(H:H)=1,'Student List'!D1,ifna(xlookup($A:$A,'Student List'!$A:$A,'Student List'!D:D),)),"")</f>
         <v>Student Last Name</v>
       </c>
-      <c r="G1" s="40" t="str">
+      <c r="G1" s="37" t="str">
         <f t="array" ref="G1:G2">ifna(if(row(J:J)=1,'Student List'!E1,ifna(xlookup($A:$A,'Student List'!$A:$A,'Student List'!E:E),)),"")</f>
         <v>Grad Year</v>
       </c>
-      <c r="H1" s="30" t="str">
-        <f t="array" ref="H1:H2">if(row(H:H)=1,"Inactive",isna(vlookup(A:A,'Student List'!A:A,1,false)))</f>
+      <c r="H1" s="29" t="str">
+        <f t="array" ref="H1:H2">if(row(H:H)=1,"Inactive",ifna(not(xlookup(A:A,'Student List'!A:A,not('Student List'!G:G))),true))</f>
         <v>Inactive</v>
       </c>
-      <c r="I1" s="30" t="str">
+      <c r="I1" s="29" t="str">
         <f t="array" ref="I1:I2">if(row(I:I)=1,"New Advisor",J:J&lt;&gt;K:K)</f>
         <v>New Advisor</v>
       </c>
-      <c r="J1" s="30" t="str">
-        <f t="array" ref="J1:J2">if(row(J:J)=1,"Current Advisor",ifna(xlookup(A:A,'Advisor List'!A:A,'Advisor List'!G:G),))</f>
-        <v>Current Advisor</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>41</v>
+      <c r="J1" s="29" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("byrow(A:A,lambda(host_id,if(host_id=$A$1,""Advisor Email"",ifna(filter(Advisor_Email,Advisor_Host_ID=host_id,Advisor_Most_Likely_Advisor),))))"),"Advisor Email")</f>
+        <v>Advisor Email</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38" t="b">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="I2" s="38" t="b">
+      <c r="I2" s="35" t="b">
         <v>0</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="41"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="38"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$1:$K$2">
@@ -3061,7 +3564,7 @@
     </sortState>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{3FBFD739-53C5-42AA-9D25-C0C9F903DD50}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{C8DFF587-8138-47F6-882F-E53E2855F909}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$J$2"/>
     </customSheetView>
   </customSheetViews>
@@ -3100,41 +3603,41 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="30" t="str">
-        <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!G1,ifna(vlookup($A:$A,'Advisor List'!$F:$I,COLUMN()-2,false),)),)</f>
+      <c r="D1" s="29" t="str">
+        <f t="array" ref="D1:D2">ifna(if(row(D:D)=1,'Advisor List'!G1,ifna(vlookup($A:$A,'Advisor List'!$G:$I,COLUMN()-3,false),)),)</f>
         <v>Advisor Email</v>
       </c>
-      <c r="E1" s="30" t="str">
-        <f t="array" ref="E1:E2">ifna(if(row(E:E)=1,'Advisor List'!I1,ifna(vlookup($A:$A,'Advisor List'!$F:$I,COLUMN()-2,false),)),)</f>
+      <c r="E1" s="29" t="str">
+        <f t="array" ref="E1:E2">ifna(if(row(E:E)=1,'Advisor List'!I1,ifna(vlookup($A:$A,'Advisor List'!$G:$I,COLUMN()-2,false),)),)</f>
         <v>Advisor Last Name</v>
       </c>
-      <c r="F1" s="30" t="str">
+      <c r="F1" s="29" t="str">
         <f t="array" ref="F1:F2">if(row(F:F)=1,"Inactive",IF((A:A&lt;&gt;"ROOT")*(isna(vlookup(A:A,'Faculty List'!D:D,1,false))),TRUE,FALSE))</f>
         <v>Inactive</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="C2" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36" t="b">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3146,7 +3649,7 @@
     </sortState>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{3FBFD739-53C5-42AA-9D25-C0C9F903DD50}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{C8DFF587-8138-47F6-882F-E53E2855F909}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$F$2">
         <filterColumn colId="5">
           <filters>
@@ -3191,31 +3694,32 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="30" t="str">
-        <f t="array" ref="D1:D2">if(row(D:D)=1,"Inactive",IF((A:A&lt;&gt;"ROOT")*(isna(vlookup(A:A,'Student List'!E:E,1,false))),TRUE,FALSE))</f>
+      <c r="D1" s="29" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("byrow(A:A,lambda(form,if(form=$A$1,""Inactive"",and(form&lt;&gt;""ROOT"",isna(filter(Student_Host_ID,Student_Grad_Year=form,not(Student_Inactive)))))))"),"Inactive")</f>
         <v>Inactive</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="C2" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="36" t="b">
+      <c r="D2" s="34" t="b">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -3255,31 +3759,32 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="29" t="s">
+      <c r="A1" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="30" t="str">
-        <f t="array" ref="D1:D2">if(row(D:D)=1,"Inactive",IF((A:A&lt;&gt;"ROOT")*(isna(vlookup(A:A,'Student List'!E:E,1,false))),TRUE,FALSE))</f>
+      <c r="D1" s="29" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("byrow(A:A,lambda(form,if(form=$A$1,""Inactive"",AND(form&lt;&gt;""ROOT"",isna(filter(Student_Host_ID,Student_Grad_Year=form,not(Student_Inactive)))))))"),"Inactive")</f>
         <v>Inactive</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="C2" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="36" t="b">
+      <c r="D2" s="34" t="b">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),FALSE)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>